<commit_message>
updates, might have nan fixed
</commit_message>
<xml_diff>
--- a/Resources/1990/Master_1990.xlsx
+++ b/Resources/1990/Master_1990.xlsx
@@ -3357,10 +3357,10 @@
         <v>6.203288490284006</v>
       </c>
       <c r="BN2">
-        <v>22.92817679558011</v>
+        <v>4.41988950276243</v>
       </c>
       <c r="BO2">
-        <v>66.93548387096774</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:67">
@@ -3560,10 +3560,10 @@
         <v>11.50971599402093</v>
       </c>
       <c r="BN3">
-        <v>42.54143646408839</v>
+        <v>19.06077348066298</v>
       </c>
       <c r="BO3">
-        <v>124.1935483870968</v>
+        <v>20.16129032258064</v>
       </c>
     </row>
     <row r="4" spans="1:67">
@@ -3763,10 +3763,10 @@
         <v>11.80866965620329</v>
       </c>
       <c r="BN4">
-        <v>43.64640883977901</v>
+        <v>15.74585635359116</v>
       </c>
       <c r="BO4">
-        <v>127.4193548387097</v>
+        <v>10.48387096774194</v>
       </c>
     </row>
     <row r="5" spans="1:67">
@@ -3966,10 +3966,10 @@
         <v>12.03288490284006</v>
       </c>
       <c r="BN5">
-        <v>44.47513812154696</v>
+        <v>13.25966850828729</v>
       </c>
       <c r="BO5">
-        <v>129.8387096774194</v>
+        <v>20.16129032258064</v>
       </c>
     </row>
     <row r="6" spans="1:67">
@@ -4169,10 +4169,10 @@
         <v>10.53811659192825</v>
       </c>
       <c r="BN6">
-        <v>38.95027624309392</v>
+        <v>8.563535911602209</v>
       </c>
       <c r="BO6">
-        <v>113.7096774193548</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="7" spans="1:67">
@@ -4372,10 +4372,10 @@
         <v>13.97608370702541</v>
       </c>
       <c r="BN7">
-        <v>51.6574585635359</v>
+        <v>2.486187845303867</v>
       </c>
       <c r="BO7">
-        <v>150.8064516129032</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="8" spans="1:67">
@@ -4575,10 +4575,10 @@
         <v>6.278026905829597</v>
       </c>
       <c r="BN8">
-        <v>23.20441988950276</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO8">
-        <v>67.74193548387098</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="9" spans="1:67">
@@ -4775,10 +4775,10 @@
         <v>9.715994020926756</v>
       </c>
       <c r="BN9">
-        <v>35.91160220994475</v>
+        <v>5.524861878453039</v>
       </c>
       <c r="BO9">
-        <v>104.8387096774193</v>
+        <v>-7.258064516129033</v>
       </c>
     </row>
     <row r="10" spans="1:67">
@@ -4978,10 +4978,10 @@
         <v>11.13602391629297</v>
       </c>
       <c r="BN10">
-        <v>41.16022099447514</v>
+        <v>4.972375690607735</v>
       </c>
       <c r="BO10">
-        <v>120.1612903225807</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="11" spans="1:67">
@@ -5181,10 +5181,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN11">
-        <v>36.74033149171271</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO11">
-        <v>107.258064516129</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="12" spans="1:67">
@@ -5384,10 +5384,10 @@
         <v>10.38863976083707</v>
       </c>
       <c r="BN12">
-        <v>38.39779005524861</v>
+        <v>10.49723756906077</v>
       </c>
       <c r="BO12">
-        <v>112.0967741935484</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="13" spans="1:67">
@@ -5587,10 +5587,10 @@
         <v>11.36023916292974</v>
       </c>
       <c r="BN13">
-        <v>41.98895027624309</v>
+        <v>17.95580110497237</v>
       </c>
       <c r="BO13">
-        <v>122.5806451612903</v>
+        <v>19.35483870967742</v>
       </c>
     </row>
     <row r="14" spans="1:67">
@@ -5787,10 +5787,10 @@
         <v>12.92974588938715</v>
       </c>
       <c r="BN14">
-        <v>47.79005524861878</v>
+        <v>9.116022099447513</v>
       </c>
       <c r="BO14">
-        <v>139.5161290322581</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="15" spans="1:67">
@@ -5990,10 +5990,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN15">
-        <v>32.87292817679558</v>
+        <v>4.696132596685083</v>
       </c>
       <c r="BO15">
-        <v>95.96774193548387</v>
+        <v>-7.258064516129033</v>
       </c>
     </row>
     <row r="16" spans="1:67">
@@ -6193,10 +6193,10 @@
         <v>8.071748878923767</v>
       </c>
       <c r="BN16">
-        <v>29.83425414364641</v>
+        <v>3.038674033149171</v>
       </c>
       <c r="BO16">
-        <v>87.09677419354838</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="17" spans="1:67">
@@ -6396,10 +6396,10 @@
         <v>10.01494768310912</v>
       </c>
       <c r="BN17">
-        <v>37.01657458563536</v>
+        <v>12.70718232044199</v>
       </c>
       <c r="BO17">
-        <v>108.0645161290323</v>
+        <v>6.451612903225806</v>
       </c>
     </row>
     <row r="18" spans="1:67">
@@ -6599,10 +6599,10 @@
         <v>5.680119581464872</v>
       </c>
       <c r="BN18">
-        <v>20.99447513812154</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO18">
-        <v>61.29032258064515</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="19" spans="1:67">
@@ -6802,10 +6802,10 @@
         <v>20.254110612855</v>
       </c>
       <c r="BN19">
-        <v>74.86187845303867</v>
+        <v>47.79005524861878</v>
       </c>
       <c r="BO19">
-        <v>218.5483870967742</v>
+        <v>74.19354838709677</v>
       </c>
     </row>
     <row r="20" spans="1:67">
@@ -7005,10 +7005,10 @@
         <v>9.566517189835576</v>
       </c>
       <c r="BN20">
-        <v>35.35911602209944</v>
+        <v>4.972375690607735</v>
       </c>
       <c r="BO20">
-        <v>103.2258064516129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:67">
@@ -7208,10 +7208,10 @@
         <v>9.417040358744394</v>
       </c>
       <c r="BN21">
-        <v>34.80662983425414</v>
+        <v>4.696132596685083</v>
       </c>
       <c r="BO21">
-        <v>101.6129032258064</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="22" spans="1:67">
@@ -7411,10 +7411,10 @@
         <v>9.118086696562031</v>
       </c>
       <c r="BN22">
-        <v>33.70165745856353</v>
+        <v>5.248618784530386</v>
       </c>
       <c r="BO22">
-        <v>98.38709677419354</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="23" spans="1:67">
@@ -7614,10 +7614,10 @@
         <v>7.10014947683109</v>
       </c>
       <c r="BN23">
-        <v>26.24309392265193</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO23">
-        <v>76.61290322580645</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="24" spans="1:67">
@@ -7817,10 +7817,10 @@
         <v>12.4813153961136</v>
       </c>
       <c r="BN24">
-        <v>46.13259668508287</v>
+        <v>14.91712707182321</v>
       </c>
       <c r="BO24">
-        <v>134.6774193548387</v>
+        <v>18.54838709677419</v>
       </c>
     </row>
     <row r="25" spans="1:67">
@@ -8017,10 +8017,10 @@
         <v>7.473841554559042</v>
       </c>
       <c r="BN25">
-        <v>27.62430939226519</v>
+        <v>3.038674033149171</v>
       </c>
       <c r="BO25">
-        <v>80.64516129032258</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="26" spans="1:67">
@@ -8220,10 +8220,10 @@
         <v>16.3677130044843</v>
       </c>
       <c r="BN26">
-        <v>60.49723756906077</v>
+        <v>26.24309392265193</v>
       </c>
       <c r="BO26">
-        <v>176.6129032258064</v>
+        <v>49.19354838709677</v>
       </c>
     </row>
     <row r="27" spans="1:67">
@@ -8420,10 +8420,10 @@
         <v>2.466367713004484</v>
       </c>
       <c r="BN27">
-        <v>9.116022099447513</v>
+        <v>-1.104972375690608</v>
       </c>
       <c r="BO27">
-        <v>26.61290322580645</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="28" spans="1:67">
@@ -8623,10 +8623,10 @@
         <v>12.70553064275037</v>
       </c>
       <c r="BN28">
-        <v>46.96132596685082</v>
+        <v>18.78453038674033</v>
       </c>
       <c r="BO28">
-        <v>137.0967741935484</v>
+        <v>15.32258064516129</v>
       </c>
     </row>
     <row r="29" spans="1:67">
@@ -8826,10 +8826,10 @@
         <v>8.594917787742899</v>
       </c>
       <c r="BN29">
-        <v>31.76795580110497</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO29">
-        <v>92.74193548387096</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:67">
@@ -9029,10 +9029,10 @@
         <v>12.63079222720478</v>
       </c>
       <c r="BN30">
-        <v>46.68508287292817</v>
+        <v>18.50828729281768</v>
       </c>
       <c r="BO30">
-        <v>136.2903225806452</v>
+        <v>5.64516129032258</v>
       </c>
     </row>
     <row r="31" spans="1:67">
@@ -9232,10 +9232,10 @@
         <v>5.381165919282511</v>
       </c>
       <c r="BN31">
-        <v>19.88950276243094</v>
+        <v>0</v>
       </c>
       <c r="BO31">
-        <v>58.06451612903226</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="32" spans="1:67">
@@ -9435,10 +9435,10 @@
         <v>6.576980568011958</v>
       </c>
       <c r="BN32">
-        <v>24.30939226519337</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO32">
-        <v>70.96774193548387</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="33" spans="1:67">
@@ -9638,10 +9638,10 @@
         <v>12.10762331838565</v>
       </c>
       <c r="BN33">
-        <v>44.75138121546961</v>
+        <v>12.98342541436464</v>
       </c>
       <c r="BO33">
-        <v>130.6451612903226</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="34" spans="1:67">
@@ -9841,10 +9841,10 @@
         <v>12.63079222720478</v>
       </c>
       <c r="BN34">
-        <v>46.68508287292817</v>
+        <v>0</v>
       </c>
       <c r="BO34">
-        <v>136.2903225806452</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="35" spans="1:67">
@@ -10044,10 +10044,10 @@
         <v>9.715994020926756</v>
       </c>
       <c r="BN35">
-        <v>35.91160220994475</v>
+        <v>5.524861878453039</v>
       </c>
       <c r="BO35">
-        <v>104.8387096774193</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="36" spans="1:67">
@@ -10247,10 +10247,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN36">
-        <v>36.74033149171271</v>
+        <v>10.49723756906077</v>
       </c>
       <c r="BO36">
-        <v>107.258064516129</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="37" spans="1:67">
@@ -10450,10 +10450,10 @@
         <v>10.61285500747384</v>
       </c>
       <c r="BN37">
-        <v>39.22651933701657</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO37">
-        <v>114.516129032258</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="38" spans="1:67">
@@ -10653,10 +10653,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN38">
-        <v>32.87292817679558</v>
+        <v>6.077348066298343</v>
       </c>
       <c r="BO38">
-        <v>95.96774193548387</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="39" spans="1:67">
@@ -10856,10 +10856,10 @@
         <v>9.566517189835576</v>
       </c>
       <c r="BN39">
-        <v>35.35911602209944</v>
+        <v>10.22099447513812</v>
       </c>
       <c r="BO39">
-        <v>103.2258064516129</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="40" spans="1:67">
@@ -11056,10 +11056,10 @@
         <v>-0.6726457399103138</v>
       </c>
       <c r="BN40">
-        <v>-2.486187845303867</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO40">
-        <v>-7.258064516129033</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="41" spans="1:67">
@@ -11259,10 +11259,10 @@
         <v>6.128550074738415</v>
       </c>
       <c r="BN41">
-        <v>22.65193370165745</v>
+        <v>0</v>
       </c>
       <c r="BO41">
-        <v>66.12903225806451</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="42" spans="1:67">
@@ -11459,10 +11459,10 @@
         <v>7.548579970104632</v>
       </c>
       <c r="BN42">
-        <v>27.90055248618784</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO42">
-        <v>81.45161290322579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:67">
@@ -11659,10 +11659,10 @@
         <v>6.801195814648729</v>
       </c>
       <c r="BN43">
-        <v>25.13812154696132</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO43">
-        <v>73.38709677419354</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="44" spans="1:67">
@@ -11859,10 +11859,10 @@
         <v>6.801195814648729</v>
       </c>
       <c r="BN44">
-        <v>25.13812154696132</v>
+        <v>0</v>
       </c>
       <c r="BO44">
-        <v>73.38709677419354</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:67">
@@ -12062,10 +12062,10 @@
         <v>0</v>
       </c>
       <c r="BN45">
-        <v>0</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO45">
-        <v>0</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="46" spans="1:67">
@@ -12262,10 +12262,10 @@
         <v>-3.662182361733931</v>
       </c>
       <c r="BN46">
-        <v>-13.53591160220994</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO46">
-        <v>-39.51612903225807</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="47" spans="1:67">
@@ -12462,10 +12462,10 @@
         <v>10.83707025411061</v>
       </c>
       <c r="BN47">
-        <v>40.05524861878452</v>
+        <v>18.78453038674033</v>
       </c>
       <c r="BO47">
-        <v>116.9354838709677</v>
+        <v>16.12903225806452</v>
       </c>
     </row>
     <row r="48" spans="1:67">
@@ -12662,10 +12662,10 @@
         <v>7.10014947683109</v>
       </c>
       <c r="BN48">
-        <v>26.24309392265193</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO48">
-        <v>76.61290322580645</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="49" spans="1:67">
@@ -12865,10 +12865,10 @@
         <v>12.78026905829596</v>
       </c>
       <c r="BN49">
-        <v>47.23756906077348</v>
+        <v>14.64088397790055</v>
       </c>
       <c r="BO49">
-        <v>137.9032258064516</v>
+        <v>12.09677419354839</v>
       </c>
     </row>
     <row r="50" spans="1:67">
@@ -13065,10 +13065,10 @@
         <v>-6.87593423019432</v>
       </c>
       <c r="BN50">
-        <v>-25.41436464088397</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO50">
-        <v>-74.19354838709677</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="51" spans="1:67">
@@ -13268,10 +13268,10 @@
         <v>12.25710014947683</v>
       </c>
       <c r="BN51">
-        <v>45.3038674033149</v>
+        <v>9.668508287292816</v>
       </c>
       <c r="BO51">
-        <v>132.258064516129</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="52" spans="1:67">
@@ -13471,10 +13471,10 @@
         <v>9.417040358744394</v>
       </c>
       <c r="BN52">
-        <v>34.80662983425414</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO52">
-        <v>101.6129032258064</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="53" spans="1:67">
@@ -13671,10 +13671,10 @@
         <v>9.566517189835576</v>
       </c>
       <c r="BN53">
-        <v>35.35911602209944</v>
+        <v>12.43093922651934</v>
       </c>
       <c r="BO53">
-        <v>103.2258064516129</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="54" spans="1:67">
@@ -13874,10 +13874,10 @@
         <v>11.21076233183856</v>
       </c>
       <c r="BN54">
-        <v>41.43646408839778</v>
+        <v>6.906077348066297</v>
       </c>
       <c r="BO54">
-        <v>120.9677419354839</v>
+        <v>-7.258064516129033</v>
       </c>
     </row>
     <row r="55" spans="1:67">
@@ -14077,10 +14077,10 @@
         <v>15.6203288490284</v>
       </c>
       <c r="BN55">
-        <v>57.73480662983425</v>
+        <v>30.93922651933701</v>
       </c>
       <c r="BO55">
-        <v>168.5483870967742</v>
+        <v>23.38709677419355</v>
       </c>
     </row>
     <row r="56" spans="1:67">
@@ -14280,10 +14280,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN56">
-        <v>32.87292817679558</v>
+        <v>-1.933701657458563</v>
       </c>
       <c r="BO56">
-        <v>95.96774193548387</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="57" spans="1:67">
@@ -14483,10 +14483,10 @@
         <v>11.13602391629297</v>
       </c>
       <c r="BN57">
-        <v>41.16022099447514</v>
+        <v>19.61325966850828</v>
       </c>
       <c r="BO57">
-        <v>120.1612903225807</v>
+        <v>13.70967741935484</v>
       </c>
     </row>
     <row r="58" spans="1:67">
@@ -14686,10 +14686,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN58">
-        <v>36.74033149171271</v>
+        <v>3.314917127071823</v>
       </c>
       <c r="BO58">
-        <v>107.258064516129</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="59" spans="1:67">
@@ -14889,10 +14889,10 @@
         <v>9.118086696562031</v>
       </c>
       <c r="BN59">
-        <v>33.70165745856353</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO59">
-        <v>98.38709677419354</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="60" spans="1:67">
@@ -15092,10 +15092,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN60">
-        <v>43.92265193370166</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO60">
-        <v>128.2258064516129</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="61" spans="1:67">
@@ -15295,10 +15295,10 @@
         <v>9.566517189835576</v>
       </c>
       <c r="BN61">
-        <v>35.35911602209944</v>
+        <v>10.22099447513812</v>
       </c>
       <c r="BO61">
-        <v>103.2258064516129</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="62" spans="1:67">
@@ -15498,10 +15498,10 @@
         <v>7.17488789237668</v>
       </c>
       <c r="BN62">
-        <v>26.51933701657459</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO62">
-        <v>77.41935483870968</v>
+        <v>6.451612903225806</v>
       </c>
     </row>
     <row r="63" spans="1:67">
@@ -15701,10 +15701,10 @@
         <v>7.922272047832585</v>
       </c>
       <c r="BN63">
-        <v>29.2817679558011</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO63">
-        <v>85.48387096774192</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="64" spans="1:67">
@@ -15904,10 +15904,10 @@
         <v>7.473841554559042</v>
       </c>
       <c r="BN64">
-        <v>27.62430939226519</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO64">
-        <v>80.64516129032258</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="65" spans="1:67">
@@ -16107,10 +16107,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN65">
-        <v>43.92265193370166</v>
+        <v>18.78453038674033</v>
       </c>
       <c r="BO65">
-        <v>128.2258064516129</v>
+        <v>28.2258064516129</v>
       </c>
     </row>
     <row r="66" spans="1:67">
@@ -16307,10 +16307,10 @@
         <v>2.391629297458894</v>
       </c>
       <c r="BN66">
-        <v>8.839779005524861</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO66">
-        <v>25.80645161290322</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="67" spans="1:67">
@@ -16507,10 +16507,10 @@
         <v>7.847533632286995</v>
       </c>
       <c r="BN67">
-        <v>29.00552486187845</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO67">
-        <v>84.67741935483872</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="68" spans="1:67">
@@ -16710,10 +16710,10 @@
         <v>14.64872944693572</v>
       </c>
       <c r="BN68">
-        <v>54.14364640883977</v>
+        <v>24.03314917127071</v>
       </c>
       <c r="BO68">
-        <v>158.0645161290323</v>
+        <v>21.7741935483871</v>
       </c>
     </row>
     <row r="69" spans="1:67">
@@ -16913,10 +16913,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN69">
-        <v>43.92265193370166</v>
+        <v>4.972375690607735</v>
       </c>
       <c r="BO69">
-        <v>128.2258064516129</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="70" spans="1:67">
@@ -17116,10 +17116,10 @@
         <v>7.473841554559042</v>
       </c>
       <c r="BN70">
-        <v>27.62430939226519</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO70">
-        <v>80.64516129032258</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="71" spans="1:67">
@@ -17319,10 +17319,10 @@
         <v>11.50971599402093</v>
       </c>
       <c r="BN71">
-        <v>42.54143646408839</v>
+        <v>8.563535911602209</v>
       </c>
       <c r="BO71">
-        <v>124.1935483870968</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="72" spans="1:67">
@@ -17522,10 +17522,10 @@
         <v>11.95814648729447</v>
       </c>
       <c r="BN72">
-        <v>44.19889502762431</v>
+        <v>8.563535911602209</v>
       </c>
       <c r="BO72">
-        <v>129.0322580645161</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="73" spans="1:67">
@@ -17725,10 +17725,10 @@
         <v>10.23916292974589</v>
       </c>
       <c r="BN73">
-        <v>37.84530386740331</v>
+        <v>8.011049723756905</v>
       </c>
       <c r="BO73">
-        <v>110.4838709677419</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="74" spans="1:67">
@@ -17928,10 +17928,10 @@
         <v>5.007473841554559</v>
       </c>
       <c r="BN74">
-        <v>18.50828729281768</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO74">
-        <v>54.03225806451613</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="75" spans="1:67">
@@ -18131,10 +18131,10 @@
         <v>6.726457399103139</v>
       </c>
       <c r="BN75">
-        <v>24.86187845303867</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO75">
-        <v>72.58064516129032</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="76" spans="1:67">
@@ -18334,10 +18334,10 @@
         <v>13.67713004484305</v>
       </c>
       <c r="BN76">
-        <v>50.5524861878453</v>
+        <v>9.94475138121547</v>
       </c>
       <c r="BO76">
-        <v>147.5806451612903</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="77" spans="1:67">
@@ -18537,10 +18537,10 @@
         <v>11.95814648729447</v>
       </c>
       <c r="BN77">
-        <v>44.19889502762431</v>
+        <v>17.67955801104972</v>
       </c>
       <c r="BO77">
-        <v>129.0322580645161</v>
+        <v>13.70967741935484</v>
       </c>
     </row>
     <row r="78" spans="1:67">
@@ -18740,10 +18740,10 @@
         <v>9.417040358744394</v>
       </c>
       <c r="BN78">
-        <v>34.80662983425414</v>
+        <v>6.077348066298343</v>
       </c>
       <c r="BO78">
-        <v>101.6129032258064</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="79" spans="1:67">
@@ -18943,10 +18943,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN79">
-        <v>30.11049723756906</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO79">
-        <v>87.90322580645162</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="80" spans="1:67">
@@ -19146,10 +19146,10 @@
         <v>13.07922272047833</v>
       </c>
       <c r="BN80">
-        <v>48.34254143646409</v>
+        <v>13.81215469613259</v>
       </c>
       <c r="BO80">
-        <v>141.1290322580645</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="81" spans="1:67">
@@ -19346,10 +19346,10 @@
         <v>9.118086696562031</v>
       </c>
       <c r="BN81">
-        <v>33.70165745856353</v>
+        <v>12.43093922651934</v>
       </c>
       <c r="BO81">
-        <v>98.38709677419354</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="82" spans="1:67">
@@ -19549,10 +19549,10 @@
         <v>12.70553064275037</v>
       </c>
       <c r="BN82">
-        <v>46.96132596685082</v>
+        <v>12.15469613259669</v>
       </c>
       <c r="BO82">
-        <v>137.0967741935484</v>
+        <v>9.67741935483871</v>
       </c>
     </row>
     <row r="83" spans="1:67">
@@ -19752,10 +19752,10 @@
         <v>3.811659192825111</v>
       </c>
       <c r="BN83">
-        <v>14.08839779005525</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO83">
-        <v>41.12903225806451</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="84" spans="1:67">
@@ -19952,10 +19952,10 @@
         <v>4.484304932735426</v>
       </c>
       <c r="BN84">
-        <v>16.57458563535911</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO84">
-        <v>48.38709677419354</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="85" spans="1:67">
@@ -20155,10 +20155,10 @@
         <v>7.623318385650222</v>
       </c>
       <c r="BN85">
-        <v>28.17679558011049</v>
+        <v>3.867403314917126</v>
       </c>
       <c r="BO85">
-        <v>82.25806451612902</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="86" spans="1:67">
@@ -20358,10 +20358,10 @@
         <v>16.59192825112108</v>
       </c>
       <c r="BN86">
-        <v>61.32596685082872</v>
+        <v>32.04419889502762</v>
       </c>
       <c r="BO86">
-        <v>179.0322580645161</v>
+        <v>53.2258064516129</v>
       </c>
     </row>
     <row r="87" spans="1:67">
@@ -20558,10 +20558,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN87">
-        <v>36.74033149171271</v>
+        <v>13.25966850828729</v>
       </c>
       <c r="BO87">
-        <v>107.258064516129</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="88" spans="1:67">
@@ -20758,10 +20758,10 @@
         <v>7.10014947683109</v>
       </c>
       <c r="BN88">
-        <v>26.24309392265193</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO88">
-        <v>76.61290322580645</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="89" spans="1:67">
@@ -20961,10 +20961,10 @@
         <v>12.85500747384155</v>
       </c>
       <c r="BN89">
-        <v>47.51381215469613</v>
+        <v>24.03314917127071</v>
       </c>
       <c r="BO89">
-        <v>138.7096774193548</v>
+        <v>18.54838709677419</v>
       </c>
     </row>
     <row r="90" spans="1:67">
@@ -21164,10 +21164,10 @@
         <v>3.811659192825111</v>
       </c>
       <c r="BN90">
-        <v>14.08839779005525</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO90">
-        <v>41.12903225806451</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="91" spans="1:67">
@@ -21367,10 +21367,10 @@
         <v>7.324364723467862</v>
       </c>
       <c r="BN91">
-        <v>27.07182320441989</v>
+        <v>3.867403314917126</v>
       </c>
       <c r="BO91">
-        <v>79.03225806451614</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="92" spans="1:67">
@@ -21570,10 +21570,10 @@
         <v>10.68759342301943</v>
       </c>
       <c r="BN92">
-        <v>39.50276243093923</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO92">
-        <v>115.3225806451613</v>
+        <v>-7.258064516129033</v>
       </c>
     </row>
     <row r="93" spans="1:67">
@@ -21770,10 +21770,10 @@
         <v>7.922272047832585</v>
       </c>
       <c r="BN93">
-        <v>29.2817679558011</v>
+        <v>14.64088397790055</v>
       </c>
       <c r="BO93">
-        <v>85.48387096774192</v>
+        <v>18.54838709677419</v>
       </c>
     </row>
     <row r="94" spans="1:67">
@@ -21973,10 +21973,10 @@
         <v>7.997010463378175</v>
       </c>
       <c r="BN94">
-        <v>29.55801104972375</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO94">
-        <v>86.29032258064515</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="95" spans="1:67">
@@ -22176,10 +22176,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN95">
-        <v>36.74033149171271</v>
+        <v>15.4696132596685</v>
       </c>
       <c r="BO95">
-        <v>107.258064516129</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="96" spans="1:67">
@@ -22379,10 +22379,10 @@
         <v>5.829596412556053</v>
       </c>
       <c r="BN96">
-        <v>21.54696132596685</v>
+        <v>0</v>
       </c>
       <c r="BO96">
-        <v>62.90322580645162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:67">
@@ -22582,10 +22582,10 @@
         <v>8.66965620328849</v>
       </c>
       <c r="BN97">
-        <v>32.04419889502762</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO97">
-        <v>93.54838709677419</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="98" spans="1:67">
@@ -22785,10 +22785,10 @@
         <v>10.83707025411061</v>
       </c>
       <c r="BN98">
-        <v>40.05524861878452</v>
+        <v>17.95580110497237</v>
       </c>
       <c r="BO98">
-        <v>116.9354838709677</v>
+        <v>27.41935483870968</v>
       </c>
     </row>
     <row r="99" spans="1:67">
@@ -22988,10 +22988,10 @@
         <v>9.342301943198803</v>
       </c>
       <c r="BN99">
-        <v>34.53038674033149</v>
+        <v>12.70718232044199</v>
       </c>
       <c r="BO99">
-        <v>100.8064516129032</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="100" spans="1:67">
@@ -23191,10 +23191,10 @@
         <v>14.20029895366218</v>
       </c>
       <c r="BN100">
-        <v>52.48618784530387</v>
+        <v>17.67955801104972</v>
       </c>
       <c r="BO100">
-        <v>153.2258064516129</v>
+        <v>18.54838709677419</v>
       </c>
     </row>
     <row r="101" spans="1:67">
@@ -23394,10 +23394,10 @@
         <v>7.698056801195814</v>
       </c>
       <c r="BN101">
-        <v>28.45303867403315</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO101">
-        <v>83.06451612903226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:67">
@@ -23597,10 +23597,10 @@
         <v>13.37817638266069</v>
       </c>
       <c r="BN102">
-        <v>49.44751381215469</v>
+        <v>14.08839779005525</v>
       </c>
       <c r="BO102">
-        <v>144.3548387096774</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="103" spans="1:67">
@@ -23800,10 +23800,10 @@
         <v>19.28251121076233</v>
       </c>
       <c r="BN103">
-        <v>71.27071823204419</v>
+        <v>37.29281767955801</v>
       </c>
       <c r="BO103">
-        <v>208.0645161290323</v>
+        <v>41.93548387096774</v>
       </c>
     </row>
     <row r="104" spans="1:67">
@@ -24003,10 +24003,10 @@
         <v>11.58445440956652</v>
       </c>
       <c r="BN104">
-        <v>42.81767955801104</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO104">
-        <v>125</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="105" spans="1:67">
@@ -24206,10 +24206,10 @@
         <v>6.053811659192824</v>
       </c>
       <c r="BN105">
-        <v>22.3756906077348</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO105">
-        <v>65.32258064516128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:67">
@@ -24409,10 +24409,10 @@
         <v>12.18236173393124</v>
       </c>
       <c r="BN106">
-        <v>45.02762430939226</v>
+        <v>18.50828729281768</v>
       </c>
       <c r="BO106">
-        <v>131.4516129032258</v>
+        <v>16.12903225806452</v>
       </c>
     </row>
     <row r="107" spans="1:67">
@@ -24612,10 +24612,10 @@
         <v>10.61285500747384</v>
       </c>
       <c r="BN107">
-        <v>39.22651933701657</v>
+        <v>17.40331491712707</v>
       </c>
       <c r="BO107">
-        <v>114.516129032258</v>
+        <v>6.451612903225806</v>
       </c>
     </row>
     <row r="108" spans="1:67">
@@ -24812,10 +24812,10 @@
         <v>8.295964125560538</v>
       </c>
       <c r="BN108">
-        <v>30.66298342541436</v>
+        <v>5.524861878453039</v>
       </c>
       <c r="BO108">
-        <v>89.51612903225806</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="109" spans="1:67">
@@ -25015,10 +25015,10 @@
         <v>4.633781763826607</v>
       </c>
       <c r="BN109">
-        <v>17.12707182320442</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO109">
-        <v>50</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="110" spans="1:67">
@@ -25218,10 +25218,10 @@
         <v>9.192825112107624</v>
       </c>
       <c r="BN110">
-        <v>33.97790055248619</v>
+        <v>5.248618784530386</v>
       </c>
       <c r="BO110">
-        <v>99.19354838709677</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="111" spans="1:67">
@@ -25421,10 +25421,10 @@
         <v>7.324364723467862</v>
       </c>
       <c r="BN111">
-        <v>27.07182320441989</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO111">
-        <v>79.03225806451614</v>
+        <v>-6.451612903225806</v>
       </c>
     </row>
     <row r="112" spans="1:67">
@@ -25624,10 +25624,10 @@
         <v>8.819133034379671</v>
       </c>
       <c r="BN112">
-        <v>32.59668508287293</v>
+        <v>6.906077348066297</v>
       </c>
       <c r="BO112">
-        <v>95.16129032258065</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="113" spans="1:67">
@@ -25827,10 +25827,10 @@
         <v>9.641255605381167</v>
       </c>
       <c r="BN113">
-        <v>35.63535911602209</v>
+        <v>4.143646408839778</v>
       </c>
       <c r="BO113">
-        <v>104.0322580645161</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="114" spans="1:67">
@@ -26030,10 +26030,10 @@
         <v>17.11509715994021</v>
       </c>
       <c r="BN114">
-        <v>63.25966850828728</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO114">
-        <v>184.6774193548387</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="115" spans="1:67">
@@ -26233,10 +26233,10 @@
         <v>12.40657698056801</v>
       </c>
       <c r="BN115">
-        <v>45.85635359116022</v>
+        <v>12.43093922651934</v>
       </c>
       <c r="BO115">
-        <v>133.8709677419355</v>
+        <v>8.870967741935484</v>
       </c>
     </row>
     <row r="116" spans="1:67">
@@ -26436,10 +26436,10 @@
         <v>11.7339312406577</v>
       </c>
       <c r="BN116">
-        <v>43.37016574585635</v>
+        <v>16.57458563535911</v>
       </c>
       <c r="BO116">
-        <v>126.6129032258064</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="117" spans="1:67">
@@ -26639,10 +26639,10 @@
         <v>11.43497757847534</v>
       </c>
       <c r="BN117">
-        <v>42.26519337016575</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO117">
-        <v>123.3870967741936</v>
+        <v>6.451612903225806</v>
       </c>
     </row>
     <row r="118" spans="1:67">
@@ -26842,10 +26842,10 @@
         <v>7.24962630792227</v>
       </c>
       <c r="BN118">
-        <v>26.79558011049724</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO118">
-        <v>78.2258064516129</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="119" spans="1:67">
@@ -27045,10 +27045,10 @@
         <v>8.968609865470851</v>
       </c>
       <c r="BN119">
-        <v>33.14917127071823</v>
+        <v>7.18232044198895</v>
       </c>
       <c r="BO119">
-        <v>96.77419354838709</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="120" spans="1:67">
@@ -27245,10 +27245,10 @@
         <v>12.40657698056801</v>
       </c>
       <c r="BN120">
-        <v>45.85635359116022</v>
+        <v>22.09944751381216</v>
       </c>
       <c r="BO120">
-        <v>133.8709677419355</v>
+        <v>23.38709677419355</v>
       </c>
     </row>
     <row r="121" spans="1:67">
@@ -27448,10 +27448,10 @@
         <v>6.352765321375187</v>
       </c>
       <c r="BN121">
-        <v>23.48066298342541</v>
+        <v>1.657458563535912</v>
       </c>
       <c r="BO121">
-        <v>68.54838709677419</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="122" spans="1:67">
@@ -27651,10 +27651,10 @@
         <v>8.520179372197308</v>
       </c>
       <c r="BN122">
-        <v>31.49171270718232</v>
+        <v>4.143646408839778</v>
       </c>
       <c r="BO122">
-        <v>91.93548387096774</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="123" spans="1:67">
@@ -27854,10 +27854,10 @@
         <v>10.98654708520179</v>
       </c>
       <c r="BN123">
-        <v>40.60773480662983</v>
+        <v>21.2707182320442</v>
       </c>
       <c r="BO123">
-        <v>118.5483870967742</v>
+        <v>12.90322580645161</v>
       </c>
     </row>
     <row r="124" spans="1:67">
@@ -28057,10 +28057,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN124">
-        <v>30.11049723756906</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO124">
-        <v>87.90322580645162</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="125" spans="1:67">
@@ -28260,10 +28260,10 @@
         <v>9.491778774289985</v>
       </c>
       <c r="BN125">
-        <v>35.08287292817679</v>
+        <v>4.696132596685083</v>
       </c>
       <c r="BO125">
-        <v>102.4193548387097</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="126" spans="1:67">
@@ -28460,10 +28460,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN126">
-        <v>30.11049723756906</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO126">
-        <v>87.90322580645162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:67">
@@ -28663,10 +28663,10 @@
         <v>10.1644245142003</v>
       </c>
       <c r="BN127">
-        <v>37.56906077348066</v>
+        <v>6.906077348066297</v>
       </c>
       <c r="BO127">
-        <v>109.6774193548387</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="128" spans="1:67">
@@ -28866,10 +28866,10 @@
         <v>6.203288490284006</v>
       </c>
       <c r="BN128">
-        <v>22.92817679558011</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO128">
-        <v>66.93548387096774</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="129" spans="1:67">
@@ -29069,10 +29069,10 @@
         <v>6.352765321375187</v>
       </c>
       <c r="BN129">
-        <v>23.48066298342541</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO129">
-        <v>68.54838709677419</v>
+        <v>-10.48387096774194</v>
       </c>
     </row>
     <row r="130" spans="1:67">
@@ -29272,10 +29272,10 @@
         <v>7.847533632286995</v>
       </c>
       <c r="BN130">
-        <v>29.00552486187845</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO130">
-        <v>84.67741935483872</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="131" spans="1:67">
@@ -29475,10 +29475,10 @@
         <v>6.352765321375187</v>
       </c>
       <c r="BN131">
-        <v>23.48066298342541</v>
+        <v>7.734806629834252</v>
       </c>
       <c r="BO131">
-        <v>68.54838709677419</v>
+        <v>8.870967741935484</v>
       </c>
     </row>
     <row r="132" spans="1:67">
@@ -29678,10 +29678,10 @@
         <v>7.698056801195814</v>
       </c>
       <c r="BN132">
-        <v>28.45303867403315</v>
+        <v>8.011049723756905</v>
       </c>
       <c r="BO132">
-        <v>83.06451612903226</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="133" spans="1:67">
@@ -29881,10 +29881,10 @@
         <v>11.95814648729447</v>
       </c>
       <c r="BN133">
-        <v>44.19889502762431</v>
+        <v>9.116022099447513</v>
       </c>
       <c r="BO133">
-        <v>129.0322580645161</v>
+        <v>10.48387096774194</v>
       </c>
     </row>
     <row r="134" spans="1:67">
@@ -30084,10 +30084,10 @@
         <v>14.7982062780269</v>
       </c>
       <c r="BN134">
-        <v>54.69613259668508</v>
+        <v>27.34806629834254</v>
       </c>
       <c r="BO134">
-        <v>159.6774193548387</v>
+        <v>38.70967741935484</v>
       </c>
     </row>
     <row r="135" spans="1:67">
@@ -30287,10 +30287,10 @@
         <v>15.09715994020926</v>
       </c>
       <c r="BN135">
-        <v>55.80110497237568</v>
+        <v>10.77348066298342</v>
       </c>
       <c r="BO135">
-        <v>162.9032258064516</v>
+        <v>17.74193548387097</v>
       </c>
     </row>
     <row r="136" spans="1:67">
@@ -30487,10 +30487,10 @@
         <v>4.484304932735426</v>
       </c>
       <c r="BN136">
-        <v>16.57458563535911</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO136">
-        <v>48.38709677419354</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="137" spans="1:67">
@@ -30690,10 +30690,10 @@
         <v>5.23168908819133</v>
       </c>
       <c r="BN137">
-        <v>19.33701657458563</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO137">
-        <v>56.4516129032258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:67">
@@ -30893,10 +30893,10 @@
         <v>12.70553064275037</v>
       </c>
       <c r="BN138">
-        <v>46.96132596685082</v>
+        <v>22.09944751381216</v>
       </c>
       <c r="BO138">
-        <v>137.0967741935484</v>
+        <v>23.38709677419355</v>
       </c>
     </row>
     <row r="139" spans="1:67">
@@ -31096,10 +31096,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN139">
-        <v>32.87292817679558</v>
+        <v>3.314917127071823</v>
       </c>
       <c r="BO139">
-        <v>95.96774193548387</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="140" spans="1:67">
@@ -31296,10 +31296,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN140">
-        <v>30.11049723756906</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO140">
-        <v>87.90322580645162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:67">
@@ -31499,10 +31499,10 @@
         <v>11.58445440956652</v>
       </c>
       <c r="BN141">
-        <v>42.81767955801104</v>
+        <v>13.81215469613259</v>
       </c>
       <c r="BO141">
-        <v>125</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="142" spans="1:67">
@@ -31699,10 +31699,10 @@
         <v>11.36023916292974</v>
       </c>
       <c r="BN142">
-        <v>41.98895027624309</v>
+        <v>4.972375690607735</v>
       </c>
       <c r="BO142">
-        <v>122.5806451612903</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="143" spans="1:67">
@@ -31902,10 +31902,10 @@
         <v>9.342301943198803</v>
       </c>
       <c r="BN143">
-        <v>34.53038674033149</v>
+        <v>7.18232044198895</v>
       </c>
       <c r="BO143">
-        <v>100.8064516129032</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="144" spans="1:67">
@@ -32102,10 +32102,10 @@
         <v>2.167414050822122</v>
       </c>
       <c r="BN144">
-        <v>8.011049723756905</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO144">
-        <v>23.38709677419355</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="145" spans="1:67">
@@ -32302,10 +32302,10 @@
         <v>5.754857997010463</v>
       </c>
       <c r="BN145">
-        <v>21.2707182320442</v>
+        <v>0</v>
       </c>
       <c r="BO145">
-        <v>62.09677419354838</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="146" spans="1:67">
@@ -32505,10 +32505,10 @@
         <v>10.1644245142003</v>
       </c>
       <c r="BN146">
-        <v>37.56906077348066</v>
+        <v>8.563535911602209</v>
       </c>
       <c r="BO146">
-        <v>109.6774193548387</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="147" spans="1:67">
@@ -32705,10 +32705,10 @@
         <v>3.811659192825111</v>
       </c>
       <c r="BN147">
-        <v>14.08839779005525</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO147">
-        <v>41.12903225806451</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="148" spans="1:67">
@@ -32908,10 +32908,10 @@
         <v>14.64872944693572</v>
       </c>
       <c r="BN148">
-        <v>54.14364640883977</v>
+        <v>24.03314917127071</v>
       </c>
       <c r="BO148">
-        <v>158.0645161290323</v>
+        <v>33.06451612903226</v>
       </c>
     </row>
     <row r="149" spans="1:67">
@@ -33111,10 +33111,10 @@
         <v>10.83707025411061</v>
       </c>
       <c r="BN149">
-        <v>40.05524861878452</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO149">
-        <v>116.9354838709677</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="150" spans="1:67">
@@ -33314,10 +33314,10 @@
         <v>6.203288490284006</v>
       </c>
       <c r="BN150">
-        <v>22.92817679558011</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO150">
-        <v>66.93548387096774</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="151" spans="1:67">
@@ -33517,10 +33517,10 @@
         <v>12.25710014947683</v>
       </c>
       <c r="BN151">
-        <v>45.3038674033149</v>
+        <v>20.99447513812154</v>
       </c>
       <c r="BO151">
-        <v>132.258064516129</v>
+        <v>20.16129032258064</v>
       </c>
     </row>
     <row r="152" spans="1:67">
@@ -33720,10 +33720,10 @@
         <v>11.65919282511211</v>
       </c>
       <c r="BN152">
-        <v>43.0939226519337</v>
+        <v>3.314917127071823</v>
       </c>
       <c r="BO152">
-        <v>125.8064516129032</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="153" spans="1:67">
@@ -33923,10 +33923,10 @@
         <v>8.071748878923767</v>
       </c>
       <c r="BN153">
-        <v>29.83425414364641</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO153">
-        <v>87.09677419354838</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="154" spans="1:67">
@@ -34126,10 +34126,10 @@
         <v>10.68759342301943</v>
       </c>
       <c r="BN154">
-        <v>39.50276243093923</v>
+        <v>10.22099447513812</v>
       </c>
       <c r="BO154">
-        <v>115.3225806451613</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="155" spans="1:67">
@@ -34329,10 +34329,10 @@
         <v>6.053811659192824</v>
       </c>
       <c r="BN155">
-        <v>22.3756906077348</v>
+        <v>0</v>
       </c>
       <c r="BO155">
-        <v>65.32258064516128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:67">
@@ -34532,10 +34532,10 @@
         <v>8.66965620328849</v>
       </c>
       <c r="BN156">
-        <v>32.04419889502762</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO156">
-        <v>93.54838709677419</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="157" spans="1:67">
@@ -34735,10 +34735,10 @@
         <v>9.641255605381167</v>
       </c>
       <c r="BN157">
-        <v>35.63535911602209</v>
+        <v>17.12707182320442</v>
       </c>
       <c r="BO157">
-        <v>104.0322580645161</v>
+        <v>14.51612903225807</v>
       </c>
     </row>
     <row r="158" spans="1:67">
@@ -34938,10 +34938,10 @@
         <v>9.267563527653214</v>
       </c>
       <c r="BN158">
-        <v>34.25414364640883</v>
+        <v>10.49723756906077</v>
       </c>
       <c r="BO158">
-        <v>100</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="159" spans="1:67">
@@ -35141,10 +35141,10 @@
         <v>11.13602391629297</v>
       </c>
       <c r="BN159">
-        <v>41.16022099447514</v>
+        <v>10.77348066298342</v>
       </c>
       <c r="BO159">
-        <v>120.1612903225807</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="160" spans="1:67">
@@ -35344,10 +35344,10 @@
         <v>3.43796711509716</v>
       </c>
       <c r="BN160">
-        <v>12.70718232044199</v>
+        <v>-1.104972375690608</v>
       </c>
       <c r="BO160">
-        <v>37.09677419354838</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="161" spans="1:67">
@@ -35547,10 +35547,10 @@
         <v>17.04035874439462</v>
       </c>
       <c r="BN161">
-        <v>62.98342541436463</v>
+        <v>32.04419889502762</v>
       </c>
       <c r="BO161">
-        <v>183.8709677419355</v>
+        <v>32.25806451612903</v>
       </c>
     </row>
     <row r="162" spans="1:67">
@@ -35750,10 +35750,10 @@
         <v>19.88041853512705</v>
       </c>
       <c r="BN162">
-        <v>73.48066298342542</v>
+        <v>45.58011049723756</v>
       </c>
       <c r="BO162">
-        <v>214.516129032258</v>
+        <v>68.54838709677419</v>
       </c>
     </row>
     <row r="163" spans="1:67">
@@ -35953,10 +35953,10 @@
         <v>6.352765321375187</v>
       </c>
       <c r="BN163">
-        <v>23.48066298342541</v>
+        <v>0</v>
       </c>
       <c r="BO163">
-        <v>68.54838709677419</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="164" spans="1:67">
@@ -36153,10 +36153,10 @@
         <v>7.17488789237668</v>
       </c>
       <c r="BN164">
-        <v>26.51933701657459</v>
+        <v>0</v>
       </c>
       <c r="BO164">
-        <v>77.41935483870968</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="165" spans="1:67">
@@ -36356,10 +36356,10 @@
         <v>9.641255605381167</v>
       </c>
       <c r="BN165">
-        <v>35.63535911602209</v>
+        <v>8.839779005524861</v>
       </c>
       <c r="BO165">
-        <v>104.0322580645161</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="166" spans="1:67">
@@ -36559,10 +36559,10 @@
         <v>10.53811659192825</v>
       </c>
       <c r="BN166">
-        <v>38.95027624309392</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO166">
-        <v>113.7096774193548</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="167" spans="1:67">
@@ -36762,10 +36762,10 @@
         <v>5.680119581464872</v>
       </c>
       <c r="BN167">
-        <v>20.99447513812154</v>
+        <v>0</v>
       </c>
       <c r="BO167">
-        <v>61.29032258064515</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="168" spans="1:67">
@@ -36965,10 +36965,10 @@
         <v>5.381165919282511</v>
       </c>
       <c r="BN168">
-        <v>19.88950276243094</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO168">
-        <v>58.06451612903226</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="169" spans="1:67">
@@ -37165,10 +37165,10 @@
         <v>6.87593423019432</v>
       </c>
       <c r="BN169">
-        <v>25.41436464088397</v>
+        <v>10.49723756906077</v>
       </c>
       <c r="BO169">
-        <v>74.19354838709677</v>
+        <v>16.93548387096774</v>
       </c>
     </row>
     <row r="170" spans="1:67">
@@ -37368,10 +37368,10 @@
         <v>23.31838565022421</v>
       </c>
       <c r="BN170">
-        <v>86.18784530386739</v>
+        <v>52.48618784530387</v>
       </c>
       <c r="BO170">
-        <v>251.6129032258065</v>
+        <v>81.45161290322579</v>
       </c>
     </row>
     <row r="171" spans="1:67">
@@ -37571,10 +37571,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN171">
-        <v>43.92265193370166</v>
+        <v>5.801104972375691</v>
       </c>
       <c r="BO171">
-        <v>128.2258064516129</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="172" spans="1:67">
@@ -37774,10 +37774,10 @@
         <v>7.997010463378175</v>
       </c>
       <c r="BN172">
-        <v>29.55801104972375</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO172">
-        <v>86.29032258064515</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="173" spans="1:67">
@@ -37977,10 +37977,10 @@
         <v>8.968609865470851</v>
       </c>
       <c r="BN173">
-        <v>33.14917127071823</v>
+        <v>8.839779005524861</v>
       </c>
       <c r="BO173">
-        <v>96.77419354838709</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="174" spans="1:67">
@@ -38180,10 +38180,10 @@
         <v>11.7339312406577</v>
       </c>
       <c r="BN174">
-        <v>43.37016574585635</v>
+        <v>24.30939226519337</v>
       </c>
       <c r="BO174">
-        <v>126.6129032258064</v>
+        <v>29.03225806451613</v>
       </c>
     </row>
     <row r="175" spans="1:67">
@@ -38383,10 +38383,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN175">
-        <v>30.11049723756906</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO175">
-        <v>87.90322580645162</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="176" spans="1:67">
@@ -38583,10 +38583,10 @@
         <v>9.043348281016442</v>
       </c>
       <c r="BN176">
-        <v>33.42541436464088</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO176">
-        <v>97.58064516129032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:67">
@@ -38786,10 +38786,10 @@
         <v>14.050822122571</v>
       </c>
       <c r="BN177">
-        <v>51.93370165745856</v>
+        <v>15.19337016574586</v>
       </c>
       <c r="BO177">
-        <v>151.6129032258065</v>
+        <v>12.09677419354839</v>
       </c>
     </row>
     <row r="178" spans="1:67">
@@ -38989,10 +38989,10 @@
         <v>10.31390134529148</v>
       </c>
       <c r="BN178">
-        <v>38.12154696132596</v>
+        <v>9.94475138121547</v>
       </c>
       <c r="BO178">
-        <v>111.2903225806452</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="179" spans="1:67">
@@ -39192,10 +39192,10 @@
         <v>5.23168908819133</v>
       </c>
       <c r="BN179">
-        <v>19.33701657458563</v>
+        <v>2.209944751381215</v>
       </c>
       <c r="BO179">
-        <v>56.4516129032258</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="180" spans="1:67">
@@ -39395,10 +39395,10 @@
         <v>7.847533632286995</v>
       </c>
       <c r="BN180">
-        <v>29.00552486187845</v>
+        <v>6.353591160220994</v>
       </c>
       <c r="BO180">
-        <v>84.67741935483872</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="181" spans="1:67">
@@ -39598,10 +39598,10 @@
         <v>6.502242152466367</v>
       </c>
       <c r="BN181">
-        <v>24.03314917127071</v>
+        <v>3.867403314917126</v>
       </c>
       <c r="BO181">
-        <v>70.16129032258064</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="182" spans="1:67">
@@ -39801,10 +39801,10 @@
         <v>4.559043348281016</v>
       </c>
       <c r="BN182">
-        <v>16.85082872928177</v>
+        <v>0</v>
       </c>
       <c r="BO182">
-        <v>49.19354838709677</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="183" spans="1:67">
@@ -40004,10 +40004,10 @@
         <v>5.680119581464872</v>
       </c>
       <c r="BN183">
-        <v>20.99447513812154</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO183">
-        <v>61.29032258064515</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="184" spans="1:67">
@@ -40207,10 +40207,10 @@
         <v>11.80866965620329</v>
       </c>
       <c r="BN184">
-        <v>43.64640883977901</v>
+        <v>27.90055248618784</v>
       </c>
       <c r="BO184">
-        <v>127.4193548387097</v>
+        <v>31.45161290322581</v>
       </c>
     </row>
     <row r="185" spans="1:67">
@@ -40410,10 +40410,10 @@
         <v>9.566517189835576</v>
       </c>
       <c r="BN185">
-        <v>35.35911602209944</v>
+        <v>3.314917127071823</v>
       </c>
       <c r="BO185">
-        <v>103.2258064516129</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="186" spans="1:67">
@@ -40610,10 +40610,10 @@
         <v>9.865470852017935</v>
       </c>
       <c r="BN186">
-        <v>36.46408839779005</v>
+        <v>8.287292817679557</v>
       </c>
       <c r="BO186">
-        <v>106.4516129032258</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="187" spans="1:67">
@@ -40810,10 +40810,10 @@
         <v>4.334828101644245</v>
       </c>
       <c r="BN187">
-        <v>16.02209944751381</v>
+        <v>0</v>
       </c>
       <c r="BO187">
-        <v>46.7741935483871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:67">
@@ -41010,10 +41010,10 @@
         <v>9.043348281016442</v>
       </c>
       <c r="BN188">
-        <v>33.42541436464088</v>
+        <v>4.696132596685083</v>
       </c>
       <c r="BO188">
-        <v>97.58064516129032</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="189" spans="1:67">
@@ -41213,10 +41213,10 @@
         <v>5.007473841554559</v>
       </c>
       <c r="BN189">
-        <v>18.50828729281768</v>
+        <v>0</v>
       </c>
       <c r="BO189">
-        <v>54.03225806451613</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="190" spans="1:67">
@@ -41416,10 +41416,10 @@
         <v>4.633781763826607</v>
       </c>
       <c r="BN190">
-        <v>17.12707182320442</v>
+        <v>0</v>
       </c>
       <c r="BO190">
-        <v>50</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="191" spans="1:67">
@@ -41619,10 +41619,10 @@
         <v>6.95067264573991</v>
       </c>
       <c r="BN191">
-        <v>25.69060773480663</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO191">
-        <v>75</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="192" spans="1:67">
@@ -41816,10 +41816,10 @@
         <v>-6.726457399103139</v>
       </c>
       <c r="BN192">
-        <v>-24.86187845303867</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO192">
-        <v>-72.58064516129032</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="193" spans="1:67">
@@ -42019,10 +42019,10 @@
         <v>14.87294469357249</v>
       </c>
       <c r="BN193">
-        <v>54.97237569060772</v>
+        <v>24.30939226519337</v>
       </c>
       <c r="BO193">
-        <v>160.4838709677419</v>
+        <v>43.54838709677419</v>
       </c>
     </row>
     <row r="194" spans="1:67">
@@ -42222,10 +42222,10 @@
         <v>9.043348281016442</v>
       </c>
       <c r="BN194">
-        <v>33.42541436464088</v>
+        <v>9.392265193370166</v>
       </c>
       <c r="BO194">
-        <v>97.58064516129032</v>
+        <v>8.870967741935484</v>
       </c>
     </row>
     <row r="195" spans="1:67">
@@ -42422,10 +42422,10 @@
         <v>9.865470852017935</v>
       </c>
       <c r="BN195">
-        <v>36.46408839779005</v>
+        <v>0</v>
       </c>
       <c r="BO195">
-        <v>106.4516129032258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:67">
@@ -42625,10 +42625,10 @@
         <v>12.55605381165919</v>
       </c>
       <c r="BN196">
-        <v>46.40883977900553</v>
+        <v>18.50828729281768</v>
       </c>
       <c r="BO196">
-        <v>135.483870967742</v>
+        <v>16.93548387096774</v>
       </c>
     </row>
     <row r="197" spans="1:67">
@@ -42828,10 +42828,10 @@
         <v>9.192825112107624</v>
       </c>
       <c r="BN197">
-        <v>33.97790055248619</v>
+        <v>4.972375690607735</v>
       </c>
       <c r="BO197">
-        <v>99.19354838709677</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="198" spans="1:67">
@@ -43031,10 +43031,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN198">
-        <v>30.11049723756906</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO198">
-        <v>87.90322580645162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:67">
@@ -43231,10 +43231,10 @@
         <v>8.66965620328849</v>
       </c>
       <c r="BN199">
-        <v>32.04419889502762</v>
+        <v>0</v>
       </c>
       <c r="BO199">
-        <v>93.54838709677419</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="200" spans="1:67">
@@ -43434,10 +43434,10 @@
         <v>10.1644245142003</v>
       </c>
       <c r="BN200">
-        <v>37.56906077348066</v>
+        <v>9.116022099447513</v>
       </c>
       <c r="BO200">
-        <v>109.6774193548387</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="201" spans="1:67">
@@ -43637,10 +43637,10 @@
         <v>8.66965620328849</v>
       </c>
       <c r="BN201">
-        <v>32.04419889502762</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO201">
-        <v>93.54838709677419</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="202" spans="1:67">
@@ -43840,10 +43840,10 @@
         <v>7.997010463378175</v>
       </c>
       <c r="BN202">
-        <v>29.55801104972375</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO202">
-        <v>86.29032258064515</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="203" spans="1:67">
@@ -44043,10 +44043,10 @@
         <v>6.502242152466367</v>
       </c>
       <c r="BN203">
-        <v>24.03314917127071</v>
+        <v>4.143646408839778</v>
       </c>
       <c r="BO203">
-        <v>70.16129032258064</v>
+        <v>-8.064516129032258</v>
       </c>
     </row>
     <row r="204" spans="1:67">
@@ -44246,10 +44246,10 @@
         <v>8.594917787742899</v>
       </c>
       <c r="BN204">
-        <v>31.76795580110497</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO204">
-        <v>92.74193548387096</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="205" spans="1:67">
@@ -44449,10 +44449,10 @@
         <v>10.38863976083707</v>
       </c>
       <c r="BN205">
-        <v>38.39779005524861</v>
+        <v>14.64088397790055</v>
       </c>
       <c r="BO205">
-        <v>112.0967741935484</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="206" spans="1:67">
@@ -44652,10 +44652,10 @@
         <v>10.08968609865471</v>
       </c>
       <c r="BN206">
-        <v>37.29281767955801</v>
+        <v>15.19337016574586</v>
       </c>
       <c r="BO206">
-        <v>108.8709677419355</v>
+        <v>20.16129032258064</v>
       </c>
     </row>
     <row r="207" spans="1:67">
@@ -44855,10 +44855,10 @@
         <v>13.82660687593423</v>
       </c>
       <c r="BN207">
-        <v>51.10497237569061</v>
+        <v>14.3646408839779</v>
       </c>
       <c r="BO207">
-        <v>149.1935483870968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:67">
@@ -45058,10 +45058,10 @@
         <v>20.32884902840059</v>
       </c>
       <c r="BN208">
-        <v>75.13812154696133</v>
+        <v>43.92265193370166</v>
       </c>
       <c r="BO208">
-        <v>219.3548387096774</v>
+        <v>54.03225806451613</v>
       </c>
     </row>
     <row r="209" spans="1:67">
@@ -45261,10 +45261,10 @@
         <v>15.09715994020926</v>
       </c>
       <c r="BN209">
-        <v>55.80110497237568</v>
+        <v>21.2707182320442</v>
       </c>
       <c r="BO209">
-        <v>162.9032258064516</v>
+        <v>16.93548387096774</v>
       </c>
     </row>
     <row r="210" spans="1:67">
@@ -45464,10 +45464,10 @@
         <v>12.18236173393124</v>
       </c>
       <c r="BN210">
-        <v>45.02762430939226</v>
+        <v>14.64088397790055</v>
       </c>
       <c r="BO210">
-        <v>131.4516129032258</v>
+        <v>15.32258064516129</v>
       </c>
     </row>
     <row r="211" spans="1:67">
@@ -45667,10 +45667,10 @@
         <v>4.110612855007473</v>
       </c>
       <c r="BN211">
-        <v>15.19337016574586</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO211">
-        <v>44.35483870967742</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="212" spans="1:67">
@@ -45870,10 +45870,10 @@
         <v>11.58445440956652</v>
       </c>
       <c r="BN212">
-        <v>42.81767955801104</v>
+        <v>10.49723756906077</v>
       </c>
       <c r="BO212">
-        <v>125</v>
+        <v>5.64516129032258</v>
       </c>
     </row>
     <row r="213" spans="1:67">
@@ -46073,10 +46073,10 @@
         <v>6.502242152466367</v>
       </c>
       <c r="BN213">
-        <v>24.03314917127071</v>
+        <v>2.486187845303867</v>
       </c>
       <c r="BO213">
-        <v>70.16129032258064</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="214" spans="1:67">
@@ -46273,10 +46273,10 @@
         <v>5.156950672645739</v>
       </c>
       <c r="BN214">
-        <v>19.06077348066298</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO214">
-        <v>55.64516129032258</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="215" spans="1:67">
@@ -46476,10 +46476,10 @@
         <v>14.64872944693572</v>
       </c>
       <c r="BN215">
-        <v>54.14364640883977</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO215">
-        <v>158.0645161290323</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:67">
@@ -46679,10 +46679,10 @@
         <v>8.594917787742899</v>
       </c>
       <c r="BN216">
-        <v>31.76795580110497</v>
+        <v>7.734806629834252</v>
       </c>
       <c r="BO216">
-        <v>92.74193548387096</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="217" spans="1:67">
@@ -46879,10 +46879,10 @@
         <v>9.267563527653214</v>
       </c>
       <c r="BN217">
-        <v>34.25414364640883</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO217">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:67">
@@ -47079,10 +47079,10 @@
         <v>3.811659192825111</v>
       </c>
       <c r="BN218">
-        <v>14.08839779005525</v>
+        <v>0</v>
       </c>
       <c r="BO218">
-        <v>41.12903225806451</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="219" spans="1:67">
@@ -47282,10 +47282,10 @@
         <v>3.43796711509716</v>
       </c>
       <c r="BN219">
-        <v>12.70718232044199</v>
+        <v>-1.933701657458563</v>
       </c>
       <c r="BO219">
-        <v>37.09677419354838</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="220" spans="1:67">
@@ -47482,10 +47482,10 @@
         <v>1.943198804185351</v>
       </c>
       <c r="BN220">
-        <v>7.18232044198895</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO220">
-        <v>20.96774193548387</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="221" spans="1:67">
@@ -47685,10 +47685,10 @@
         <v>12.4813153961136</v>
       </c>
       <c r="BN221">
-        <v>46.13259668508287</v>
+        <v>21.8232044198895</v>
       </c>
       <c r="BO221">
-        <v>134.6774193548387</v>
+        <v>29.03225806451613</v>
       </c>
     </row>
     <row r="222" spans="1:67">
@@ -47888,10 +47888,10 @@
         <v>13.37817638266069</v>
       </c>
       <c r="BN222">
-        <v>49.44751381215469</v>
+        <v>14.91712707182321</v>
       </c>
       <c r="BO222">
-        <v>144.3548387096774</v>
+        <v>15.32258064516129</v>
       </c>
     </row>
     <row r="223" spans="1:67">
@@ -48091,10 +48091,10 @@
         <v>7.324364723467862</v>
       </c>
       <c r="BN223">
-        <v>27.07182320441989</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO223">
-        <v>79.03225806451614</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:67">
@@ -48294,10 +48294,10 @@
         <v>16.29297458893871</v>
       </c>
       <c r="BN224">
-        <v>60.22099447513812</v>
+        <v>30.66298342541436</v>
       </c>
       <c r="BO224">
-        <v>175.8064516129032</v>
+        <v>31.45161290322581</v>
       </c>
     </row>
     <row r="225" spans="1:67">
@@ -48497,10 +48497,10 @@
         <v>11.65919282511211</v>
       </c>
       <c r="BN225">
-        <v>43.0939226519337</v>
+        <v>17.40331491712707</v>
       </c>
       <c r="BO225">
-        <v>125.8064516129032</v>
+        <v>22.58064516129032</v>
       </c>
     </row>
     <row r="226" spans="1:67">
@@ -48700,10 +48700,10 @@
         <v>0.4484304932735425</v>
       </c>
       <c r="BN226">
-        <v>1.657458563535912</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO226">
-        <v>4.838709677419355</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="227" spans="1:67">
@@ -48903,10 +48903,10 @@
         <v>10.76233183856502</v>
       </c>
       <c r="BN227">
-        <v>39.77900552486188</v>
+        <v>13.53591160220994</v>
       </c>
       <c r="BO227">
-        <v>116.1290322580645</v>
+        <v>24.19354838709677</v>
       </c>
     </row>
     <row r="228" spans="1:67">
@@ -49103,10 +49103,10 @@
         <v>8.445440956651719</v>
       </c>
       <c r="BN228">
-        <v>31.21546961325967</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO228">
-        <v>91.12903225806453</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="229" spans="1:67">
@@ -49303,10 +49303,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN229">
-        <v>32.87292817679558</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO229">
-        <v>95.96774193548387</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="230" spans="1:67">
@@ -49506,10 +49506,10 @@
         <v>15.54559043348281</v>
       </c>
       <c r="BN230">
-        <v>57.4585635359116</v>
+        <v>33.42541436464088</v>
       </c>
       <c r="BO230">
-        <v>167.741935483871</v>
+        <v>37.09677419354838</v>
       </c>
     </row>
     <row r="231" spans="1:67">
@@ -49709,10 +49709,10 @@
         <v>10.23916292974589</v>
       </c>
       <c r="BN231">
-        <v>37.84530386740331</v>
+        <v>14.08839779005525</v>
       </c>
       <c r="BO231">
-        <v>110.4838709677419</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="232" spans="1:67">
@@ -49912,10 +49912,10 @@
         <v>5.754857997010463</v>
       </c>
       <c r="BN232">
-        <v>21.2707182320442</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO232">
-        <v>62.09677419354838</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="233" spans="1:67">
@@ -50115,10 +50115,10 @@
         <v>6.053811659192824</v>
       </c>
       <c r="BN233">
-        <v>22.3756906077348</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO233">
-        <v>65.32258064516128</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="234" spans="1:67">
@@ -50318,10 +50318,10 @@
         <v>11.06128550074738</v>
       </c>
       <c r="BN234">
-        <v>40.88397790055249</v>
+        <v>8.839779005524861</v>
       </c>
       <c r="BO234">
-        <v>119.3548387096774</v>
+        <v>14.51612903225807</v>
       </c>
     </row>
     <row r="235" spans="1:67">
@@ -50521,10 +50521,10 @@
         <v>3.139013452914798</v>
       </c>
       <c r="BN235">
-        <v>11.60220994475138</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO235">
-        <v>33.87096774193549</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="236" spans="1:67">
@@ -50724,10 +50724,10 @@
         <v>4.409566517189836</v>
       </c>
       <c r="BN236">
-        <v>16.29834254143647</v>
+        <v>-2.486187845303867</v>
       </c>
       <c r="BO236">
-        <v>47.58064516129033</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="237" spans="1:67">
@@ -50927,10 +50927,10 @@
         <v>16.96562032884903</v>
       </c>
       <c r="BN237">
-        <v>62.70718232044198</v>
+        <v>28.17679558011049</v>
       </c>
       <c r="BO237">
-        <v>183.0645161290323</v>
+        <v>39.51612903225807</v>
       </c>
     </row>
     <row r="238" spans="1:67">
@@ -51130,10 +51130,10 @@
         <v>9.715994020926756</v>
       </c>
       <c r="BN238">
-        <v>35.91160220994475</v>
+        <v>16.85082872928177</v>
       </c>
       <c r="BO238">
-        <v>104.8387096774193</v>
+        <v>12.90322580645161</v>
       </c>
     </row>
     <row r="239" spans="1:67">
@@ -51333,10 +51333,10 @@
         <v>7.324364723467862</v>
       </c>
       <c r="BN239">
-        <v>27.07182320441989</v>
+        <v>0</v>
       </c>
       <c r="BO239">
-        <v>79.03225806451614</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="240" spans="1:67">
@@ -51536,10 +51536,10 @@
         <v>14.27503736920777</v>
       </c>
       <c r="BN240">
-        <v>52.76243093922653</v>
+        <v>17.95580110497237</v>
       </c>
       <c r="BO240">
-        <v>154.0322580645161</v>
+        <v>20.16129032258064</v>
       </c>
     </row>
     <row r="241" spans="1:67">
@@ -51736,10 +51736,10 @@
         <v>10.76233183856502</v>
       </c>
       <c r="BN241">
-        <v>39.77900552486188</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO241">
-        <v>116.1290322580645</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:67">
@@ -51939,10 +51939,10 @@
         <v>8.295964125560538</v>
       </c>
       <c r="BN242">
-        <v>30.66298342541436</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO242">
-        <v>89.51612903225806</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="243" spans="1:67">
@@ -52136,10 +52136,10 @@
         <v>9.043348281016442</v>
       </c>
       <c r="BN243">
-        <v>33.42541436464088</v>
+        <v>0</v>
       </c>
       <c r="BO243">
-        <v>97.58064516129032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:67">
@@ -52339,10 +52339,10 @@
         <v>9.491778774289985</v>
       </c>
       <c r="BN244">
-        <v>35.08287292817679</v>
+        <v>12.43093922651934</v>
       </c>
       <c r="BO244">
-        <v>102.4193548387097</v>
+        <v>5.64516129032258</v>
       </c>
     </row>
     <row r="245" spans="1:67">
@@ -52542,10 +52542,10 @@
         <v>5.904334828101645</v>
       </c>
       <c r="BN245">
-        <v>21.8232044198895</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO245">
-        <v>63.70967741935484</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="246" spans="1:67">
@@ -52742,10 +52742,10 @@
         <v>6.128550074738415</v>
       </c>
       <c r="BN246">
-        <v>22.65193370165745</v>
+        <v>0</v>
       </c>
       <c r="BO246">
-        <v>66.12903225806451</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="247" spans="1:67">
@@ -52945,10 +52945,10 @@
         <v>10.9118086696562</v>
       </c>
       <c r="BN247">
-        <v>40.33149171270718</v>
+        <v>8.011049723756905</v>
       </c>
       <c r="BO247">
-        <v>117.7419354838709</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="248" spans="1:67">
@@ -53148,10 +53148,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN248">
-        <v>43.92265193370166</v>
+        <v>16.57458563535911</v>
       </c>
       <c r="BO248">
-        <v>128.2258064516129</v>
+        <v>16.93548387096774</v>
       </c>
     </row>
     <row r="249" spans="1:67">
@@ -53351,10 +53351,10 @@
         <v>18.0119581464873</v>
       </c>
       <c r="BN249">
-        <v>66.57458563535911</v>
+        <v>30.93922651933701</v>
       </c>
       <c r="BO249">
-        <v>194.3548387096774</v>
+        <v>50.80645161290322</v>
       </c>
     </row>
     <row r="250" spans="1:67">
@@ -53551,10 +53551,10 @@
         <v>5.979073243647234</v>
       </c>
       <c r="BN250">
-        <v>22.09944751381216</v>
+        <v>0</v>
       </c>
       <c r="BO250">
-        <v>64.51612903225806</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="251" spans="1:67">
@@ -53754,10 +53754,10 @@
         <v>11.95814648729447</v>
       </c>
       <c r="BN251">
-        <v>44.19889502762431</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO251">
-        <v>129.0322580645161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:67">
@@ -53954,10 +53954,10 @@
         <v>14.34977578475336</v>
       </c>
       <c r="BN252">
-        <v>53.03867403314917</v>
+        <v>21.54696132596685</v>
       </c>
       <c r="BO252">
-        <v>154.8387096774194</v>
+        <v>16.93548387096774</v>
       </c>
     </row>
     <row r="253" spans="1:67">
@@ -54157,10 +54157,10 @@
         <v>3.213751868460388</v>
       </c>
       <c r="BN253">
-        <v>11.87845303867403</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO253">
-        <v>34.6774193548387</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="254" spans="1:67">
@@ -54360,10 +54360,10 @@
         <v>7.24962630792227</v>
       </c>
       <c r="BN254">
-        <v>26.79558011049724</v>
+        <v>3.867403314917126</v>
       </c>
       <c r="BO254">
-        <v>78.2258064516129</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="255" spans="1:67">
@@ -54563,10 +54563,10 @@
         <v>9.491778774289985</v>
       </c>
       <c r="BN255">
-        <v>35.08287292817679</v>
+        <v>13.25966850828729</v>
       </c>
       <c r="BO255">
-        <v>102.4193548387097</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="256" spans="1:67">
@@ -54766,10 +54766,10 @@
         <v>7.997010463378175</v>
       </c>
       <c r="BN256">
-        <v>29.55801104972375</v>
+        <v>0</v>
       </c>
       <c r="BO256">
-        <v>86.29032258064515</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="257" spans="1:67">
@@ -54969,10 +54969,10 @@
         <v>6.801195814648729</v>
       </c>
       <c r="BN257">
-        <v>25.13812154696132</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO257">
-        <v>73.38709677419354</v>
+        <v>-6.451612903225806</v>
       </c>
     </row>
     <row r="258" spans="1:67">
@@ -55172,10 +55172,10 @@
         <v>12.92974588938715</v>
       </c>
       <c r="BN258">
-        <v>47.79005524861878</v>
+        <v>22.3756906077348</v>
       </c>
       <c r="BO258">
-        <v>139.5161290322581</v>
+        <v>26.61290322580645</v>
       </c>
     </row>
     <row r="259" spans="1:67">
@@ -55375,10 +55375,10 @@
         <v>10.08968609865471</v>
       </c>
       <c r="BN259">
-        <v>37.29281767955801</v>
+        <v>3.314917127071823</v>
       </c>
       <c r="BO259">
-        <v>108.8709677419355</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="260" spans="1:67">
@@ -55578,10 +55578,10 @@
         <v>12.40657698056801</v>
       </c>
       <c r="BN260">
-        <v>45.85635359116022</v>
+        <v>14.91712707182321</v>
       </c>
       <c r="BO260">
-        <v>133.8709677419355</v>
+        <v>12.09677419354839</v>
       </c>
     </row>
     <row r="261" spans="1:67">
@@ -55781,10 +55781,10 @@
         <v>6.726457399103139</v>
       </c>
       <c r="BN261">
-        <v>24.86187845303867</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO261">
-        <v>72.58064516129032</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="262" spans="1:67">
@@ -55984,10 +55984,10 @@
         <v>11.58445440956652</v>
       </c>
       <c r="BN262">
-        <v>42.81767955801104</v>
+        <v>7.734806629834252</v>
       </c>
       <c r="BO262">
-        <v>125</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="263" spans="1:67">
@@ -56187,10 +56187,10 @@
         <v>16.3677130044843</v>
       </c>
       <c r="BN263">
-        <v>60.49723756906077</v>
+        <v>16.02209944751381</v>
       </c>
       <c r="BO263">
-        <v>176.6129032258064</v>
+        <v>8.870967741935484</v>
       </c>
     </row>
     <row r="264" spans="1:67">
@@ -56390,10 +56390,10 @@
         <v>10.23916292974589</v>
       </c>
       <c r="BN264">
-        <v>37.84530386740331</v>
+        <v>8.011049723756905</v>
       </c>
       <c r="BO264">
-        <v>110.4838709677419</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="265" spans="1:67">
@@ -56593,10 +56593,10 @@
         <v>12.18236173393124</v>
       </c>
       <c r="BN265">
-        <v>45.02762430939226</v>
+        <v>15.74585635359116</v>
       </c>
       <c r="BO265">
-        <v>131.4516129032258</v>
+        <v>29.03225806451613</v>
       </c>
     </row>
     <row r="266" spans="1:67">
@@ -56796,10 +56796,10 @@
         <v>9.267563527653214</v>
       </c>
       <c r="BN266">
-        <v>34.25414364640883</v>
+        <v>6.906077348066297</v>
       </c>
       <c r="BO266">
-        <v>100</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="267" spans="1:67">
@@ -56999,10 +56999,10 @@
         <v>14.94768310911808</v>
       </c>
       <c r="BN267">
-        <v>55.24861878453038</v>
+        <v>32.32044198895027</v>
       </c>
       <c r="BO267">
-        <v>161.2903225806452</v>
+        <v>35.48387096774194</v>
       </c>
     </row>
     <row r="268" spans="1:67">
@@ -57202,10 +57202,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN268">
-        <v>43.92265193370166</v>
+        <v>8.287292817679557</v>
       </c>
       <c r="BO268">
-        <v>128.2258064516129</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="269" spans="1:67">
@@ -57405,10 +57405,10 @@
         <v>10.23916292974589</v>
       </c>
       <c r="BN269">
-        <v>37.84530386740331</v>
+        <v>6.353591160220994</v>
       </c>
       <c r="BO269">
-        <v>110.4838709677419</v>
+        <v>5.64516129032258</v>
       </c>
     </row>
     <row r="270" spans="1:67">
@@ -57608,10 +57608,10 @@
         <v>15.76980568011958</v>
       </c>
       <c r="BN270">
-        <v>58.28729281767956</v>
+        <v>27.90055248618784</v>
       </c>
       <c r="BO270">
-        <v>170.1612903225806</v>
+        <v>32.25806451612903</v>
       </c>
     </row>
     <row r="271" spans="1:67">
@@ -57811,10 +57811,10 @@
         <v>2.914798206278026</v>
       </c>
       <c r="BN271">
-        <v>10.77348066298342</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO271">
-        <v>31.45161290322581</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="272" spans="1:67">
@@ -58014,10 +58014,10 @@
         <v>9.043348281016442</v>
       </c>
       <c r="BN272">
-        <v>33.42541436464088</v>
+        <v>11.32596685082873</v>
       </c>
       <c r="BO272">
-        <v>97.58064516129032</v>
+        <v>17.74193548387097</v>
       </c>
     </row>
     <row r="273" spans="1:67">
@@ -58217,10 +58217,10 @@
         <v>11.95814648729447</v>
       </c>
       <c r="BN273">
-        <v>44.19889502762431</v>
+        <v>14.3646408839779</v>
       </c>
       <c r="BO273">
-        <v>129.0322580645161</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="274" spans="1:67">
@@ -58420,10 +58420,10 @@
         <v>7.623318385650222</v>
       </c>
       <c r="BN274">
-        <v>28.17679558011049</v>
+        <v>3.038674033149171</v>
       </c>
       <c r="BO274">
-        <v>82.25806451612902</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="275" spans="1:67">
@@ -58623,10 +58623,10 @@
         <v>5.979073243647234</v>
       </c>
       <c r="BN275">
-        <v>22.09944751381216</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO275">
-        <v>64.51612903225806</v>
+        <v>-6.451612903225806</v>
       </c>
     </row>
     <row r="276" spans="1:67">
@@ -58826,10 +58826,10 @@
         <v>10.53811659192825</v>
       </c>
       <c r="BN276">
-        <v>38.95027624309392</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO276">
-        <v>113.7096774193548</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="277" spans="1:67">
@@ -59029,10 +59029,10 @@
         <v>8.445440956651719</v>
       </c>
       <c r="BN277">
-        <v>31.21546961325967</v>
+        <v>3.867403314917126</v>
       </c>
       <c r="BO277">
-        <v>91.12903225806453</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="278" spans="1:67">
@@ -59232,10 +59232,10 @@
         <v>11.80866965620329</v>
       </c>
       <c r="BN278">
-        <v>43.64640883977901</v>
+        <v>12.15469613259669</v>
       </c>
       <c r="BO278">
-        <v>127.4193548387097</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="279" spans="1:67">
@@ -59435,10 +59435,10 @@
         <v>12.70553064275037</v>
       </c>
       <c r="BN279">
-        <v>46.96132596685082</v>
+        <v>14.3646408839779</v>
       </c>
       <c r="BO279">
-        <v>137.0967741935484</v>
+        <v>9.67741935483871</v>
       </c>
     </row>
     <row r="280" spans="1:67">
@@ -59638,10 +59638,10 @@
         <v>7.399103139013452</v>
       </c>
       <c r="BN280">
-        <v>27.34806629834254</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO280">
-        <v>79.83870967741935</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="281" spans="1:67">
@@ -59841,10 +59841,10 @@
         <v>12.85500747384155</v>
       </c>
       <c r="BN281">
-        <v>47.51381215469613</v>
+        <v>11.04972375690608</v>
       </c>
       <c r="BO281">
-        <v>138.7096774193548</v>
+        <v>19.35483870967742</v>
       </c>
     </row>
     <row r="282" spans="1:67">
@@ -60044,10 +60044,10 @@
         <v>8.66965620328849</v>
       </c>
       <c r="BN282">
-        <v>32.04419889502762</v>
+        <v>9.668508287292816</v>
       </c>
       <c r="BO282">
-        <v>93.54838709677419</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:67">
@@ -60247,10 +60247,10 @@
         <v>14.12556053811659</v>
       </c>
       <c r="BN283">
-        <v>52.20994475138121</v>
+        <v>20.71823204419889</v>
       </c>
       <c r="BO283">
-        <v>152.4193548387097</v>
+        <v>39.51612903225807</v>
       </c>
     </row>
     <row r="284" spans="1:67">
@@ -60450,10 +60450,10 @@
         <v>6.95067264573991</v>
       </c>
       <c r="BN284">
-        <v>25.69060773480663</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO284">
-        <v>75</v>
+        <v>-8.870967741935484</v>
       </c>
     </row>
     <row r="285" spans="1:67">
@@ -60653,10 +60653,10 @@
         <v>19.65620328849028</v>
       </c>
       <c r="BN285">
-        <v>72.65193370165746</v>
+        <v>41.71270718232044</v>
       </c>
       <c r="BO285">
-        <v>212.0967741935484</v>
+        <v>51.61290322580645</v>
       </c>
     </row>
     <row r="286" spans="1:67">
@@ -60856,10 +60856,10 @@
         <v>11.50971599402093</v>
       </c>
       <c r="BN286">
-        <v>42.54143646408839</v>
+        <v>25.69060773480663</v>
       </c>
       <c r="BO286">
-        <v>124.1935483870968</v>
+        <v>25.80645161290322</v>
       </c>
     </row>
     <row r="287" spans="1:67">
@@ -61059,10 +61059,10 @@
         <v>6.576980568011958</v>
       </c>
       <c r="BN287">
-        <v>24.30939226519337</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO287">
-        <v>70.96774193548387</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:67">
@@ -61262,10 +61262,10 @@
         <v>6.128550074738415</v>
       </c>
       <c r="BN288">
-        <v>22.65193370165745</v>
+        <v>1.104972375690608</v>
       </c>
       <c r="BO288">
-        <v>66.12903225806451</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="289" spans="1:67">
@@ -61465,10 +61465,10 @@
         <v>8.744394618834079</v>
       </c>
       <c r="BN289">
-        <v>32.32044198895027</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO289">
-        <v>94.35483870967741</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="290" spans="1:67">
@@ -61665,10 +61665,10 @@
         <v>9.865470852017935</v>
       </c>
       <c r="BN290">
-        <v>36.46408839779005</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO290">
-        <v>106.4516129032258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:67">
@@ -61868,10 +61868,10 @@
         <v>10.1644245142003</v>
       </c>
       <c r="BN291">
-        <v>37.56906077348066</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO291">
-        <v>109.6774193548387</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="292" spans="1:67">
@@ -62071,10 +62071,10 @@
         <v>11.36023916292974</v>
       </c>
       <c r="BN292">
-        <v>41.98895027624309</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO292">
-        <v>122.5806451612903</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="293" spans="1:67">
@@ -62274,10 +62274,10 @@
         <v>6.427503736920777</v>
       </c>
       <c r="BN293">
-        <v>23.75690607734806</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO293">
-        <v>69.35483870967741</v>
+        <v>-6.451612903225806</v>
       </c>
     </row>
     <row r="294" spans="1:67">
@@ -62477,10 +62477,10 @@
         <v>10.08968609865471</v>
       </c>
       <c r="BN294">
-        <v>37.29281767955801</v>
+        <v>16.85082872928177</v>
       </c>
       <c r="BO294">
-        <v>108.8709677419355</v>
+        <v>19.35483870967742</v>
       </c>
     </row>
     <row r="295" spans="1:67">
@@ -62680,10 +62680,10 @@
         <v>4.110612855007473</v>
       </c>
       <c r="BN295">
-        <v>15.19337016574586</v>
+        <v>-1.657458563535912</v>
       </c>
       <c r="BO295">
-        <v>44.35483870967742</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="296" spans="1:67">
@@ -62880,10 +62880,10 @@
         <v>1.868460388639761</v>
       </c>
       <c r="BN296">
-        <v>6.906077348066297</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO296">
-        <v>20.16129032258064</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="297" spans="1:67">
@@ -63083,10 +63083,10 @@
         <v>6.801195814648729</v>
       </c>
       <c r="BN297">
-        <v>25.13812154696132</v>
+        <v>2.762430939226519</v>
       </c>
       <c r="BO297">
-        <v>73.38709677419354</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="298" spans="1:67">
@@ -63286,10 +63286,10 @@
         <v>12.33183856502242</v>
       </c>
       <c r="BN298">
-        <v>45.58011049723756</v>
+        <v>12.43093922651934</v>
       </c>
       <c r="BO298">
-        <v>133.0645161290323</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="299" spans="1:67">
@@ -63489,10 +63489,10 @@
         <v>13.15396113602392</v>
       </c>
       <c r="BN299">
-        <v>48.61878453038674</v>
+        <v>22.3756906077348</v>
       </c>
       <c r="BO299">
-        <v>141.9354838709677</v>
+        <v>19.35483870967742</v>
       </c>
     </row>
     <row r="300" spans="1:67">
@@ -63692,10 +63692,10 @@
         <v>10.68759342301943</v>
       </c>
       <c r="BN300">
-        <v>39.50276243093923</v>
+        <v>16.57458563535911</v>
       </c>
       <c r="BO300">
-        <v>115.3225806451613</v>
+        <v>13.70967741935484</v>
       </c>
     </row>
     <row r="301" spans="1:67">
@@ -63895,10 +63895,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN301">
-        <v>43.92265193370166</v>
+        <v>8.839779005524861</v>
       </c>
       <c r="BO301">
-        <v>128.2258064516129</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="302" spans="1:67">
@@ -64098,10 +64098,10 @@
         <v>6.87593423019432</v>
       </c>
       <c r="BN302">
-        <v>25.41436464088397</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO302">
-        <v>74.19354838709677</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="303" spans="1:67">
@@ -64301,10 +64301,10 @@
         <v>9.192825112107624</v>
       </c>
       <c r="BN303">
-        <v>33.97790055248619</v>
+        <v>4.143646408839778</v>
       </c>
       <c r="BO303">
-        <v>99.19354838709677</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="304" spans="1:67">
@@ -64501,10 +64501,10 @@
         <v>1.868460388639761</v>
       </c>
       <c r="BN304">
-        <v>6.906077348066297</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO304">
-        <v>20.16129032258064</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="305" spans="1:67">
@@ -64704,10 +64704,10 @@
         <v>10.01494768310912</v>
       </c>
       <c r="BN305">
-        <v>37.01657458563536</v>
+        <v>9.116022099447513</v>
       </c>
       <c r="BO305">
-        <v>108.0645161290323</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="306" spans="1:67">
@@ -64904,10 +64904,10 @@
         <v>-5.082212257100148</v>
       </c>
       <c r="BN306">
-        <v>-18.78453038674033</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO306">
-        <v>-54.83870967741935</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="307" spans="1:67">
@@ -65107,10 +65107,10 @@
         <v>6.651718983557549</v>
       </c>
       <c r="BN307">
-        <v>24.58563535911602</v>
+        <v>0.5524861878453038</v>
       </c>
       <c r="BO307">
-        <v>71.7741935483871</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="308" spans="1:67">
@@ -65310,10 +65310,10 @@
         <v>10.98654708520179</v>
       </c>
       <c r="BN308">
-        <v>40.60773480662983</v>
+        <v>13.81215469613259</v>
       </c>
       <c r="BO308">
-        <v>118.5483870967742</v>
+        <v>13.70967741935484</v>
       </c>
     </row>
     <row r="309" spans="1:67">
@@ -65513,10 +65513,10 @@
         <v>9.865470852017935</v>
       </c>
       <c r="BN309">
-        <v>36.46408839779005</v>
+        <v>5.524861878453039</v>
       </c>
       <c r="BO309">
-        <v>106.4516129032258</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="310" spans="1:67">
@@ -65716,10 +65716,10 @@
         <v>14.57399103139013</v>
       </c>
       <c r="BN310">
-        <v>53.86740331491713</v>
+        <v>25.96685082872928</v>
       </c>
       <c r="BO310">
-        <v>157.258064516129</v>
+        <v>20.16129032258064</v>
       </c>
     </row>
     <row r="311" spans="1:67">
@@ -65919,10 +65919,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN311">
-        <v>36.74033149171271</v>
+        <v>3.038674033149171</v>
       </c>
       <c r="BO311">
-        <v>107.258064516129</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="312" spans="1:67">
@@ -66122,10 +66122,10 @@
         <v>10.23916292974589</v>
       </c>
       <c r="BN312">
-        <v>37.84530386740331</v>
+        <v>8.011049723756905</v>
       </c>
       <c r="BO312">
-        <v>110.4838709677419</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="313" spans="1:67">
@@ -66325,10 +66325,10 @@
         <v>9.940209267563526</v>
       </c>
       <c r="BN313">
-        <v>36.74033149171271</v>
+        <v>7.18232044198895</v>
       </c>
       <c r="BO313">
-        <v>107.258064516129</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="314" spans="1:67">
@@ -66528,10 +66528,10 @@
         <v>7.324364723467862</v>
       </c>
       <c r="BN314">
-        <v>27.07182320441989</v>
+        <v>7.18232044198895</v>
       </c>
       <c r="BO314">
-        <v>79.03225806451614</v>
+        <v>6.451612903225806</v>
       </c>
     </row>
     <row r="315" spans="1:67">
@@ -66731,10 +66731,10 @@
         <v>10.61285500747384</v>
       </c>
       <c r="BN315">
-        <v>39.22651933701657</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO315">
-        <v>114.516129032258</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="316" spans="1:67">
@@ -66934,10 +66934,10 @@
         <v>12.85500747384155</v>
       </c>
       <c r="BN316">
-        <v>47.51381215469613</v>
+        <v>9.116022099447513</v>
       </c>
       <c r="BO316">
-        <v>138.7096774193548</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="317" spans="1:67">
@@ -67137,10 +67137,10 @@
         <v>13.52765321375187</v>
       </c>
       <c r="BN317">
-        <v>50</v>
+        <v>18.23204419889503</v>
       </c>
       <c r="BO317">
-        <v>145.9677419354839</v>
+        <v>13.70967741935484</v>
       </c>
     </row>
     <row r="318" spans="1:67">
@@ -67337,10 +67337,10 @@
         <v>5.30642750373692</v>
       </c>
       <c r="BN318">
-        <v>19.61325966850828</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO318">
-        <v>57.25806451612902</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="319" spans="1:67">
@@ -67540,10 +67540,10 @@
         <v>6.576980568011958</v>
       </c>
       <c r="BN319">
-        <v>24.30939226519337</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO319">
-        <v>70.96774193548387</v>
+        <v>-11.29032258064516</v>
       </c>
     </row>
     <row r="320" spans="1:67">
@@ -67743,10 +67743,10 @@
         <v>17.86248131539611</v>
       </c>
       <c r="BN320">
-        <v>66.02209944751381</v>
+        <v>39.77900552486188</v>
       </c>
       <c r="BO320">
-        <v>192.7419354838709</v>
+        <v>36.29032258064516</v>
       </c>
     </row>
     <row r="321" spans="1:67">
@@ -67943,10 +67943,10 @@
         <v>-6.128550074738415</v>
       </c>
       <c r="BN321">
-        <v>-22.65193370165745</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO321">
-        <v>-66.12903225806451</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="322" spans="1:67">
@@ -68146,10 +68146,10 @@
         <v>11.7339312406577</v>
       </c>
       <c r="BN322">
-        <v>43.37016574585635</v>
+        <v>11.87845303867403</v>
       </c>
       <c r="BO322">
-        <v>126.6129032258064</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="323" spans="1:67">
@@ -68349,10 +68349,10 @@
         <v>8.370702541106127</v>
       </c>
       <c r="BN323">
-        <v>30.93922651933701</v>
+        <v>2.209944751381215</v>
       </c>
       <c r="BO323">
-        <v>90.32258064516128</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="324" spans="1:67">
@@ -68552,10 +68552,10 @@
         <v>13.45291479820628</v>
       </c>
       <c r="BN324">
-        <v>49.72375690607734</v>
+        <v>9.668508287292816</v>
       </c>
       <c r="BO324">
-        <v>145.1612903225806</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="325" spans="1:67">
@@ -68755,10 +68755,10 @@
         <v>7.10014947683109</v>
       </c>
       <c r="BN325">
-        <v>26.24309392265193</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO325">
-        <v>76.61290322580645</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="326" spans="1:67">
@@ -68958,10 +68958,10 @@
         <v>2.840059790732436</v>
       </c>
       <c r="BN326">
-        <v>10.49723756906077</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO326">
-        <v>30.64516129032258</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="327" spans="1:67">
@@ -69161,10 +69161,10 @@
         <v>11.06128550074738</v>
       </c>
       <c r="BN327">
-        <v>40.88397790055249</v>
+        <v>7.458563535911603</v>
       </c>
       <c r="BO327">
-        <v>119.3548387096774</v>
+        <v>-3.225806451612903</v>
       </c>
     </row>
     <row r="328" spans="1:67">
@@ -69364,10 +69364,10 @@
         <v>11.88340807174888</v>
       </c>
       <c r="BN328">
-        <v>43.92265193370166</v>
+        <v>6.906077348066297</v>
       </c>
       <c r="BO328">
-        <v>128.2258064516129</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="329" spans="1:67">
@@ -69567,10 +69567,10 @@
         <v>12.92974588938715</v>
       </c>
       <c r="BN329">
-        <v>47.79005524861878</v>
+        <v>18.50828729281768</v>
       </c>
       <c r="BO329">
-        <v>139.5161290322581</v>
+        <v>27.41935483870968</v>
       </c>
     </row>
     <row r="330" spans="1:67">
@@ -69770,10 +69770,10 @@
         <v>10.98654708520179</v>
       </c>
       <c r="BN330">
-        <v>40.60773480662983</v>
+        <v>9.94475138121547</v>
       </c>
       <c r="BO330">
-        <v>118.5483870967742</v>
+        <v>13.70967741935484</v>
       </c>
     </row>
     <row r="331" spans="1:67">
@@ -69973,10 +69973,10 @@
         <v>7.698056801195814</v>
       </c>
       <c r="BN331">
-        <v>28.45303867403315</v>
+        <v>6.629834254143646</v>
       </c>
       <c r="BO331">
-        <v>83.06451612903226</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="332" spans="1:67">
@@ -70173,10 +70173,10 @@
         <v>10.01494768310912</v>
       </c>
       <c r="BN332">
-        <v>37.01657458563536</v>
+        <v>12.98342541436464</v>
       </c>
       <c r="BO332">
-        <v>108.0645161290323</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="333" spans="1:67">
@@ -70376,10 +70376,10 @@
         <v>4.559043348281016</v>
       </c>
       <c r="BN333">
-        <v>16.85082872928177</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO333">
-        <v>49.19354838709677</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="334" spans="1:67">
@@ -70579,10 +70579,10 @@
         <v>12.03288490284006</v>
       </c>
       <c r="BN334">
-        <v>44.47513812154696</v>
+        <v>23.48066298342541</v>
       </c>
       <c r="BO334">
-        <v>129.8387096774194</v>
+        <v>25.80645161290322</v>
       </c>
     </row>
     <row r="335" spans="1:67">
@@ -70782,10 +70782,10 @@
         <v>13.00448430493273</v>
       </c>
       <c r="BN335">
-        <v>48.06629834254143</v>
+        <v>12.70718232044199</v>
       </c>
       <c r="BO335">
-        <v>140.3225806451613</v>
+        <v>9.67741935483871</v>
       </c>
     </row>
     <row r="336" spans="1:67">
@@ -70985,10 +70985,10 @@
         <v>13.52765321375187</v>
       </c>
       <c r="BN336">
-        <v>50</v>
+        <v>19.33701657458563</v>
       </c>
       <c r="BO336">
-        <v>145.9677419354839</v>
+        <v>5.64516129032258</v>
       </c>
     </row>
     <row r="337" spans="1:67">
@@ -71188,10 +71188,10 @@
         <v>10.31390134529148</v>
       </c>
       <c r="BN337">
-        <v>38.12154696132596</v>
+        <v>6.906077348066297</v>
       </c>
       <c r="BO337">
-        <v>111.2903225806452</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="338" spans="1:67">
@@ -71391,10 +71391,10 @@
         <v>5.979073243647234</v>
       </c>
       <c r="BN338">
-        <v>22.09944751381216</v>
+        <v>0</v>
       </c>
       <c r="BO338">
-        <v>64.51612903225806</v>
+        <v>-8.064516129032258</v>
       </c>
     </row>
     <row r="339" spans="1:67">
@@ -71594,10 +71594,10 @@
         <v>10.1644245142003</v>
       </c>
       <c r="BN339">
-        <v>37.56906077348066</v>
+        <v>5.801104972375691</v>
       </c>
       <c r="BO339">
-        <v>109.6774193548387</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="340" spans="1:67">
@@ -71797,10 +71797,10 @@
         <v>8.968609865470851</v>
       </c>
       <c r="BN340">
-        <v>33.14917127071823</v>
+        <v>9.116022099447513</v>
       </c>
       <c r="BO340">
-        <v>96.77419354838709</v>
+        <v>5.64516129032258</v>
       </c>
     </row>
     <row r="341" spans="1:67">
@@ -72000,10 +72000,10 @@
         <v>4.633781763826607</v>
       </c>
       <c r="BN341">
-        <v>17.12707182320442</v>
+        <v>-0.8287292817679558</v>
       </c>
       <c r="BO341">
-        <v>50</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="342" spans="1:67">
@@ -72203,10 +72203,10 @@
         <v>10.61285500747384</v>
       </c>
       <c r="BN342">
-        <v>39.22651933701657</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO342">
-        <v>114.516129032258</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="343" spans="1:67">
@@ -72406,10 +72406,10 @@
         <v>4.932735426008968</v>
       </c>
       <c r="BN343">
-        <v>18.23204419889503</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO343">
-        <v>53.2258064516129</v>
+        <v>-7.258064516129033</v>
       </c>
     </row>
     <row r="344" spans="1:67">
@@ -72609,10 +72609,10 @@
         <v>9.566517189835576</v>
       </c>
       <c r="BN344">
-        <v>35.35911602209944</v>
+        <v>4.972375690607735</v>
       </c>
       <c r="BO344">
-        <v>103.2258064516129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:67">
@@ -72812,10 +72812,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN345">
-        <v>32.87292817679558</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO345">
-        <v>95.96774193548387</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="346" spans="1:67">
@@ -73015,10 +73015,10 @@
         <v>9.342301943198803</v>
       </c>
       <c r="BN346">
-        <v>34.53038674033149</v>
+        <v>2.209944751381215</v>
       </c>
       <c r="BO346">
-        <v>100.8064516129032</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="347" spans="1:67">
@@ -73218,10 +73218,10 @@
         <v>8.819133034379671</v>
       </c>
       <c r="BN347">
-        <v>32.59668508287293</v>
+        <v>1.38121546961326</v>
       </c>
       <c r="BO347">
-        <v>95.16129032258065</v>
+        <v>-2.419354838709677</v>
       </c>
     </row>
     <row r="348" spans="1:67">
@@ -73421,10 +73421,10 @@
         <v>11.50971599402093</v>
       </c>
       <c r="BN348">
-        <v>42.54143646408839</v>
+        <v>6.629834254143646</v>
       </c>
       <c r="BO348">
-        <v>124.1935483870968</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="349" spans="1:67">
@@ -73618,10 +73618,10 @@
         <v>14.34977578475336</v>
       </c>
       <c r="BN349">
-        <v>53.03867403314917</v>
+        <v>0</v>
       </c>
       <c r="BO349">
-        <v>154.8387096774194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="350" spans="1:67">
@@ -73821,10 +73821,10 @@
         <v>8.89387144992526</v>
       </c>
       <c r="BN350">
-        <v>32.87292817679558</v>
+        <v>3.867403314917126</v>
       </c>
       <c r="BO350">
-        <v>95.96774193548387</v>
+        <v>2.419354838709677</v>
       </c>
     </row>
     <row r="351" spans="1:67">
@@ -73997,10 +73997,7 @@
         <v>15.91928251121076</v>
       </c>
       <c r="BN351">
-        <v>58.83977900552486</v>
-      </c>
-      <c r="BO351">
-        <v>171.7741935483871</v>
+        <v>-84.53038674033149</v>
       </c>
     </row>
     <row r="352" spans="1:67">
@@ -74200,10 +74197,10 @@
         <v>11.65919282511211</v>
       </c>
       <c r="BN352">
-        <v>43.0939226519337</v>
+        <v>17.40331491712707</v>
       </c>
       <c r="BO352">
-        <v>125.8064516129032</v>
+        <v>28.2258064516129</v>
       </c>
     </row>
     <row r="353" spans="1:67">
@@ -74403,10 +74400,10 @@
         <v>9.491778774289985</v>
       </c>
       <c r="BN353">
-        <v>35.08287292817679</v>
+        <v>11.04972375690608</v>
       </c>
       <c r="BO353">
-        <v>102.4193548387097</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="354" spans="1:67">
@@ -74606,10 +74603,10 @@
         <v>11.43497757847534</v>
       </c>
       <c r="BN354">
-        <v>42.26519337016575</v>
+        <v>12.43093922651934</v>
       </c>
       <c r="BO354">
-        <v>123.3870967741936</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="355" spans="1:67">
@@ -74806,10 +74803,10 @@
         <v>4.708520179372197</v>
       </c>
       <c r="BN355">
-        <v>17.40331491712707</v>
+        <v>0</v>
       </c>
       <c r="BO355">
-        <v>50.80645161290322</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="356" spans="1:67">
@@ -75009,10 +75006,10 @@
         <v>7.922272047832585</v>
       </c>
       <c r="BN356">
-        <v>29.2817679558011</v>
+        <v>3.314917127071823</v>
       </c>
       <c r="BO356">
-        <v>85.48387096774192</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="357" spans="1:67">
@@ -75212,10 +75209,10 @@
         <v>5.605381165919282</v>
       </c>
       <c r="BN357">
-        <v>20.71823204419889</v>
+        <v>-0.2762430939226519</v>
       </c>
       <c r="BO357">
-        <v>60.48387096774194</v>
+        <v>-4.032258064516129</v>
       </c>
     </row>
     <row r="358" spans="1:67">
@@ -75412,10 +75409,10 @@
         <v>11.7339312406577</v>
       </c>
       <c r="BN358">
-        <v>43.37016574585635</v>
+        <v>22.65193370165745</v>
       </c>
       <c r="BO358">
-        <v>126.6129032258064</v>
+        <v>19.35483870967742</v>
       </c>
     </row>
     <row r="359" spans="1:67">
@@ -75615,10 +75612,10 @@
         <v>5.530642750373691</v>
       </c>
       <c r="BN359">
-        <v>20.44198895027624</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO359">
-        <v>59.67741935483871</v>
+        <v>-6.451612903225806</v>
       </c>
     </row>
     <row r="360" spans="1:67">
@@ -75818,10 +75815,10 @@
         <v>12.18236173393124</v>
       </c>
       <c r="BN360">
-        <v>45.02762430939226</v>
+        <v>14.91712707182321</v>
       </c>
       <c r="BO360">
-        <v>131.4516129032258</v>
+        <v>8.064516129032258</v>
       </c>
     </row>
     <row r="361" spans="1:67">
@@ -76021,10 +76018,10 @@
         <v>8.445440956651719</v>
       </c>
       <c r="BN361">
-        <v>31.21546961325967</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO361">
-        <v>91.12903225806453</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="362" spans="1:67">
@@ -76224,10 +76221,10 @@
         <v>18.38565022421525</v>
       </c>
       <c r="BN362">
-        <v>67.95580110497238</v>
+        <v>30.66298342541436</v>
       </c>
       <c r="BO362">
-        <v>198.3870967741935</v>
+        <v>33.87096774193549</v>
       </c>
     </row>
     <row r="363" spans="1:67">
@@ -76427,10 +76424,10 @@
         <v>7.399103139013452</v>
       </c>
       <c r="BN363">
-        <v>27.34806629834254</v>
+        <v>2.209944751381215</v>
       </c>
       <c r="BO363">
-        <v>79.83870967741935</v>
+        <v>-9.67741935483871</v>
       </c>
     </row>
     <row r="364" spans="1:67">
@@ -76630,10 +76627,10 @@
         <v>10.68759342301943</v>
       </c>
       <c r="BN364">
-        <v>39.50276243093923</v>
+        <v>12.15469613259669</v>
       </c>
       <c r="BO364">
-        <v>115.3225806451613</v>
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="365" spans="1:67">
@@ -76833,10 +76830,10 @@
         <v>10.68759342301943</v>
       </c>
       <c r="BN365">
-        <v>39.50276243093923</v>
+        <v>24.03314917127071</v>
       </c>
       <c r="BO365">
-        <v>115.3225806451613</v>
+        <v>21.7741935483871</v>
       </c>
     </row>
     <row r="366" spans="1:67">
@@ -77036,10 +77033,10 @@
         <v>7.772795216741405</v>
       </c>
       <c r="BN366">
-        <v>28.7292817679558</v>
+        <v>6.077348066298343</v>
       </c>
       <c r="BO366">
-        <v>83.87096774193549</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="367" spans="1:67">
@@ -77236,10 +77233,10 @@
         <v>14.20029895366218</v>
       </c>
       <c r="BN367">
-        <v>52.48618784530387</v>
+        <v>24.03314917127071</v>
       </c>
       <c r="BO367">
-        <v>153.2258064516129</v>
+        <v>24.19354838709677</v>
       </c>
     </row>
     <row r="368" spans="1:67">
@@ -77439,10 +77436,10 @@
         <v>13.15396113602392</v>
       </c>
       <c r="BN368">
-        <v>48.61878453038674</v>
+        <v>3.591160220994475</v>
       </c>
       <c r="BO368">
-        <v>141.9354838709677</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="369" spans="1:67">
@@ -77642,10 +77639,10 @@
         <v>13.37817638266069</v>
       </c>
       <c r="BN369">
-        <v>49.44751381215469</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO369">
-        <v>144.3548387096774</v>
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="370" spans="1:67">
@@ -77845,10 +77842,10 @@
         <v>2.615844544095665</v>
       </c>
       <c r="BN370">
-        <v>9.668508287292816</v>
+        <v>0</v>
       </c>
       <c r="BO370">
-        <v>28.2258064516129</v>
+        <v>-0.8064516129032258</v>
       </c>
     </row>
     <row r="371" spans="1:67">
@@ -78048,10 +78045,10 @@
         <v>6.801195814648729</v>
       </c>
       <c r="BN371">
-        <v>25.13812154696132</v>
+        <v>0</v>
       </c>
       <c r="BO371">
-        <v>73.38709677419354</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="372" spans="1:67">
@@ -78251,10 +78248,10 @@
         <v>11.7339312406577</v>
       </c>
       <c r="BN372">
-        <v>43.37016574585635</v>
+        <v>12.98342541436464</v>
       </c>
       <c r="BO372">
-        <v>126.6129032258064</v>
+        <v>4.032258064516129</v>
       </c>
     </row>
     <row r="373" spans="1:67">
@@ -78454,10 +78451,10 @@
         <v>7.025411061285499</v>
       </c>
       <c r="BN373">
-        <v>25.96685082872928</v>
+        <v>5.248618784530386</v>
       </c>
       <c r="BO373">
-        <v>75.80645161290323</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="374" spans="1:67">
@@ -78657,10 +78654,10 @@
         <v>5.156950672645739</v>
       </c>
       <c r="BN374">
-        <v>19.06077348066298</v>
+        <v>0</v>
       </c>
       <c r="BO374">
-        <v>55.64516129032258</v>
+        <v>-4.838709677419355</v>
       </c>
     </row>
     <row r="375" spans="1:67">
@@ -78860,10 +78857,10 @@
         <v>5.082212257100148</v>
       </c>
       <c r="BN375">
-        <v>18.78453038674033</v>
+        <v>-0.5524861878453038</v>
       </c>
       <c r="BO375">
-        <v>54.83870967741935</v>
+        <v>-9.67741935483871</v>
       </c>
     </row>
     <row r="376" spans="1:67">
@@ -79063,10 +79060,10 @@
         <v>8.146487294469356</v>
       </c>
       <c r="BN376">
-        <v>30.11049723756906</v>
+        <v>0.8287292817679558</v>
       </c>
       <c r="BO376">
-        <v>87.90322580645162</v>
+        <v>-1.612903225806452</v>
       </c>
     </row>
     <row r="377" spans="1:67">
@@ -79266,10 +79263,10 @@
         <v>6.576980568011958</v>
       </c>
       <c r="BN377">
-        <v>24.30939226519337</v>
+        <v>1.933701657458563</v>
       </c>
       <c r="BO377">
-        <v>70.96774193548387</v>
+        <v>-5.64516129032258</v>
       </c>
     </row>
     <row r="378" spans="1:67">
@@ -79469,10 +79466,10 @@
         <v>13.15396113602392</v>
       </c>
       <c r="BN378">
-        <v>48.61878453038674</v>
+        <v>13.25966850828729</v>
       </c>
       <c r="BO378">
-        <v>141.9354838709677</v>
+        <v>7.258064516129033</v>
       </c>
     </row>
     <row r="379" spans="1:67">
@@ -79669,10 +79666,10 @@
         <v>19.5067264573991</v>
       </c>
       <c r="BN379">
-        <v>72.09944751381215</v>
+        <v>0.2762430939226519</v>
       </c>
       <c r="BO379">
-        <v>210.483870967742</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="380" spans="1:67">
@@ -79872,10 +79869,10 @@
         <v>14.7982062780269</v>
       </c>
       <c r="BN380">
-        <v>54.69613259668508</v>
+        <v>29.2817679558011</v>
       </c>
       <c r="BO380">
-        <v>159.6774193548387</v>
+        <v>36.29032258064516</v>
       </c>
     </row>
     <row r="381" spans="1:67">
@@ -80075,10 +80072,10 @@
         <v>8.594917787742899</v>
       </c>
       <c r="BN381">
-        <v>31.76795580110497</v>
+        <v>8.287292817679557</v>
       </c>
       <c r="BO381">
-        <v>92.74193548387096</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="382" spans="1:67">
@@ -80278,10 +80275,10 @@
         <v>11.95814648729447</v>
       </c>
       <c r="BN382">
-        <v>44.19889502762431</v>
+        <v>3.038674033149171</v>
       </c>
       <c r="BO382">
-        <v>129.0322580645161</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>